<commit_message>
wasting time on excel
</commit_message>
<xml_diff>
--- a/development/tools/PopulationCalculator.xlsx
+++ b/development/tools/PopulationCalculator.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/Documents/GitHub/Atlas-Exandria/development/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB8F2F0-4580-5449-A170-962863B80D34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95594DE3-FBD3-424C-8A4C-C7B55556CA1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="1460" windowWidth="48840" windowHeight="21520" tabRatio="918" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1580" yWindow="1460" windowWidth="48840" windowHeight="21520" tabRatio="918" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settlements" sheetId="11" r:id="rId1"/>
+    <sheet name="T-LC" sheetId="12" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="13" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Settlements!$A$2:$BO$105</definedName>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="99">
   <si>
     <t>Human</t>
   </si>
@@ -302,6 +304,30 @@
   <si>
     <t>Tabaxi Clans</t>
   </si>
+  <si>
+    <t>Duegar</t>
+  </si>
+  <si>
+    <t>Gith</t>
+  </si>
+  <si>
+    <t>Hobgonlin</t>
+  </si>
+  <si>
+    <t>Giant</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Settlement A</t>
+  </si>
+  <si>
+    <t>Major Races</t>
+  </si>
+  <si>
+    <t>Minor Races</t>
+  </si>
 </sst>
 </file>
 
@@ -312,7 +338,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,8 +368,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,6 +425,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -636,7 +720,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -692,6 +776,21 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -707,18 +806,46 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="9" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="12" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1001,11 +1128,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:BO105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="208" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18:C24"/>
+      <selection pane="bottomLeft" sqref="A1:BO33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1079,139 +1207,139 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="44"/>
       <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34" t="s">
+      <c r="G1" s="38"/>
+      <c r="H1" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34" t="s">
+      <c r="I1" s="38"/>
+      <c r="J1" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34" t="s">
+      <c r="K1" s="38"/>
+      <c r="L1" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="34"/>
-      <c r="N1" s="43" t="s">
+      <c r="M1" s="38"/>
+      <c r="N1" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40" t="s">
+      <c r="O1" s="36"/>
+      <c r="P1" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40" t="s">
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40" t="s">
+      <c r="S1" s="36"/>
+      <c r="T1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="U1" s="40"/>
-      <c r="V1" s="40" t="s">
+      <c r="U1" s="36"/>
+      <c r="V1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="40"/>
-      <c r="X1" s="34" t="s">
+      <c r="W1" s="36"/>
+      <c r="X1" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34" t="s">
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="40" t="s">
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="40" t="s">
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="40" t="s">
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="AG1" s="40"/>
-      <c r="AH1" s="34" t="s">
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="40" t="s">
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="40"/>
-      <c r="AL1" s="40" t="s">
+      <c r="AK1" s="36"/>
+      <c r="AL1" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="AM1" s="40"/>
-      <c r="AN1" s="40" t="s">
+      <c r="AM1" s="36"/>
+      <c r="AN1" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="AO1" s="40"/>
-      <c r="AP1" s="40" t="s">
+      <c r="AO1" s="36"/>
+      <c r="AP1" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="40"/>
-      <c r="AR1" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="AS1" s="40"/>
-      <c r="AT1" s="34" t="s">
+      <c r="AQ1" s="36"/>
+      <c r="AR1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS1" s="36"/>
+      <c r="AT1" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="AU1" s="34"/>
-      <c r="AV1" s="34" t="s">
+      <c r="AU1" s="38"/>
+      <c r="AV1" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="AW1" s="34"/>
-      <c r="AX1" s="34" t="s">
+      <c r="AW1" s="38"/>
+      <c r="AX1" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="AY1" s="34"/>
-      <c r="AZ1" s="34" t="s">
+      <c r="AY1" s="38"/>
+      <c r="AZ1" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="BA1" s="34"/>
-      <c r="BB1" s="34" t="s">
+      <c r="BA1" s="38"/>
+      <c r="BB1" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="BC1" s="34"/>
-      <c r="BD1" s="34" t="s">
+      <c r="BC1" s="38"/>
+      <c r="BD1" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="BE1" s="34"/>
-      <c r="BF1" s="40" t="s">
+      <c r="BE1" s="38"/>
+      <c r="BF1" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="BG1" s="41"/>
-      <c r="BH1" s="34" t="s">
+      <c r="BG1" s="45"/>
+      <c r="BH1" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="BI1" s="34"/>
-      <c r="BJ1" s="34" t="s">
+      <c r="BI1" s="38"/>
+      <c r="BJ1" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="BK1" s="34"/>
-      <c r="BL1" s="34" t="s">
+      <c r="BK1" s="38"/>
+      <c r="BL1" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="BM1" s="34"/>
-      <c r="BN1" s="35" t="s">
+      <c r="BM1" s="38"/>
+      <c r="BN1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="BO1" s="36"/>
+      <c r="BO1" s="41"/>
     </row>
     <row r="2" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
@@ -1416,7 +1544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -1651,7 +1779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -1886,7 +2014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -2121,7 +2249,7 @@
         <v>29.12</v>
       </c>
     </row>
-    <row r="6" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -2356,7 +2484,7 @@
         <v>54634.5</v>
       </c>
     </row>
-    <row r="7" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -2591,7 +2719,7 @@
         <v>50.4</v>
       </c>
     </row>
-    <row r="8" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -2826,7 +2954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -3061,7 +3189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -3296,7 +3424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -3531,7 +3659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -3766,7 +3894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
@@ -4001,7 +4129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -4236,7 +4364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -4471,7 +4599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -4706,7 +4834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
@@ -4941,7 +5069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
@@ -5176,7 +5304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -5411,7 +5539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
@@ -5646,7 +5774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -5881,7 +6009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -6116,7 +6244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
@@ -6351,7 +6479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
@@ -6601,7 +6729,7 @@
       </c>
       <c r="E25" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="11">
         <v>0</v>
@@ -6611,11 +6739,11 @@
         <v>0</v>
       </c>
       <c r="H25" s="10">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="I25" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4.46</v>
       </c>
       <c r="J25" s="10">
         <v>0</v>
@@ -6625,18 +6753,18 @@
         <v>0</v>
       </c>
       <c r="L25" s="10">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="M25" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2.23</v>
       </c>
       <c r="N25" s="11">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="O25" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4.46</v>
       </c>
       <c r="P25" s="10">
         <v>0</v>
@@ -6653,18 +6781,18 @@
         <v>0</v>
       </c>
       <c r="T25" s="10">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="U25" s="20">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>22.3</v>
       </c>
       <c r="V25" s="10">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="W25" s="20">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>89.2</v>
       </c>
       <c r="X25" s="10">
         <v>0</v>
@@ -6681,18 +6809,18 @@
         <v>0</v>
       </c>
       <c r="AB25" s="10">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="AC25" s="20">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>2.23</v>
       </c>
       <c r="AD25" s="10">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="AE25" s="20">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>178.4</v>
       </c>
       <c r="AF25" s="10">
         <v>0</v>
@@ -6702,32 +6830,32 @@
         <v>0</v>
       </c>
       <c r="AH25" s="10">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="AI25" s="20">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>2.23</v>
       </c>
       <c r="AJ25" s="10">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="AK25" s="20">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>44.6</v>
       </c>
       <c r="AL25" s="10">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="AM25" s="20">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>22.3</v>
       </c>
       <c r="AN25" s="10">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="AO25" s="20">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>178.4</v>
       </c>
       <c r="AP25" s="10">
         <v>0</v>
@@ -6737,11 +6865,11 @@
         <v>0</v>
       </c>
       <c r="AR25" s="10">
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="AS25" s="20">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1627.8999999999999</v>
       </c>
       <c r="AT25" s="10">
         <v>0</v>
@@ -6758,11 +6886,11 @@
         <v>0</v>
       </c>
       <c r="AX25" s="10">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="AY25" s="20">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>4.46</v>
       </c>
       <c r="AZ25" s="10">
         <v>0</v>
@@ -6772,25 +6900,25 @@
         <v>0</v>
       </c>
       <c r="BB25" s="10">
-        <v>0</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="BC25" s="20">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>13.38</v>
       </c>
       <c r="BD25" s="10">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="BE25" s="20">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>11.15</v>
       </c>
       <c r="BF25" s="10">
-        <v>0</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="BG25" s="20">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>24.529999999999998</v>
       </c>
       <c r="BH25" s="10">
         <v>0</v>
@@ -6836,7 +6964,7 @@
       </c>
       <c r="E26" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="11">
         <v>0</v>
@@ -6846,11 +6974,11 @@
         <v>0</v>
       </c>
       <c r="H26" s="10">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="I26" s="20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>18.03</v>
       </c>
       <c r="J26" s="10">
         <v>0</v>
@@ -6867,11 +6995,11 @@
         <v>0</v>
       </c>
       <c r="N26" s="11">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="O26" s="20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>45.075000000000003</v>
       </c>
       <c r="P26" s="10">
         <v>0</v>
@@ -6888,18 +7016,18 @@
         <v>0</v>
       </c>
       <c r="T26" s="10">
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="U26" s="20">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>108.18</v>
       </c>
       <c r="V26" s="10">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="W26" s="20">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>901.5</v>
       </c>
       <c r="X26" s="10">
         <v>0</v>
@@ -6923,11 +7051,11 @@
         <v>0</v>
       </c>
       <c r="AD26" s="10">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="AE26" s="20">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>90.15</v>
       </c>
       <c r="AF26" s="10">
         <v>0</v>
@@ -6937,32 +7065,32 @@
         <v>0</v>
       </c>
       <c r="AH26" s="10">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="AI26" s="20">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>9.0150000000000006</v>
       </c>
       <c r="AJ26" s="10">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AK26" s="20">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>450.75</v>
       </c>
       <c r="AL26" s="10">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AM26" s="20">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>45.075000000000003</v>
       </c>
       <c r="AN26" s="10">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AO26" s="20">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>901.5</v>
       </c>
       <c r="AP26" s="10">
         <v>0</v>
@@ -6972,11 +7100,11 @@
         <v>0</v>
       </c>
       <c r="AR26" s="10">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="AS26" s="20">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>6310.5</v>
       </c>
       <c r="AT26" s="10">
         <v>0</v>
@@ -6993,11 +7121,11 @@
         <v>0</v>
       </c>
       <c r="AX26" s="10">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="AY26" s="20">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>18.03</v>
       </c>
       <c r="AZ26" s="10">
         <v>0</v>
@@ -7007,32 +7135,32 @@
         <v>0</v>
       </c>
       <c r="BB26" s="10">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="BC26" s="20">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>9.0150000000000006</v>
       </c>
       <c r="BD26" s="10">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="BE26" s="20">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>18.03</v>
       </c>
       <c r="BF26" s="10">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="BG26" s="20">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>90.15</v>
       </c>
       <c r="BH26" s="10">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="BI26" s="20">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>9.0150000000000006</v>
       </c>
       <c r="BJ26" s="10">
         <v>0</v>
@@ -7071,14 +7199,14 @@
       </c>
       <c r="E27" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="11">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="G27" s="20">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="H27" s="10">
         <v>0</v>
@@ -7130,11 +7258,11 @@
         <v>0</v>
       </c>
       <c r="V27" s="10">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="W27" s="20">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="X27" s="10">
         <v>0</v>
@@ -7144,11 +7272,11 @@
         <v>0</v>
       </c>
       <c r="Z27" s="10">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="AA27" s="20">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="AB27" s="10">
         <v>0</v>
@@ -7179,11 +7307,11 @@
         <v>0</v>
       </c>
       <c r="AJ27" s="10">
-        <v>0</v>
+        <v>0.72</v>
       </c>
       <c r="AK27" s="20">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>295.2</v>
       </c>
       <c r="AL27" s="10">
         <v>0</v>
@@ -7193,11 +7321,11 @@
         <v>0</v>
       </c>
       <c r="AN27" s="10">
-        <v>0</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="AO27" s="20">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>38.950000000000003</v>
       </c>
       <c r="AP27" s="10">
         <v>0</v>
@@ -7207,11 +7335,11 @@
         <v>0</v>
       </c>
       <c r="AR27" s="10">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AS27" s="20">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="AT27" s="10">
         <v>0</v>
@@ -7256,11 +7384,11 @@
         <v>0</v>
       </c>
       <c r="BF27" s="10">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="BG27" s="20">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>20.5</v>
       </c>
       <c r="BH27" s="10">
         <v>0</v>
@@ -7306,7 +7434,7 @@
       </c>
       <c r="E28" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="11">
         <v>0</v>
@@ -7365,11 +7493,11 @@
         <v>0</v>
       </c>
       <c r="V28" s="10">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="W28" s="20">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="X28" s="10">
         <v>0</v>
@@ -7393,11 +7521,11 @@
         <v>0</v>
       </c>
       <c r="AD28" s="10">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="AE28" s="20">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>6.3</v>
       </c>
       <c r="AF28" s="10">
         <v>0</v>
@@ -7414,25 +7542,25 @@
         <v>0</v>
       </c>
       <c r="AJ28" s="10">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="AK28" s="20">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>12.6</v>
       </c>
       <c r="AL28" s="10">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="AM28" s="20">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="AN28" s="10">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AO28" s="20">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="AP28" s="10">
         <v>0</v>
@@ -7442,11 +7570,11 @@
         <v>0</v>
       </c>
       <c r="AR28" s="10">
-        <v>0</v>
+        <v>0.45</v>
       </c>
       <c r="AS28" s="20">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>94.5</v>
       </c>
       <c r="AT28" s="10">
         <v>0</v>
@@ -7463,11 +7591,11 @@
         <v>0</v>
       </c>
       <c r="AX28" s="10">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AY28" s="20">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="AZ28" s="10">
         <v>0</v>
@@ -7477,11 +7605,11 @@
         <v>0</v>
       </c>
       <c r="BB28" s="10">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="BC28" s="20">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="BD28" s="10">
         <v>0</v>
@@ -7491,18 +7619,18 @@
         <v>0</v>
       </c>
       <c r="BF28" s="10">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="BG28" s="20">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="BH28" s="10">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="BI28" s="20">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="BJ28" s="10">
         <v>0</v>
@@ -7536,9 +7664,7 @@
       <c r="C29" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D29" s="9">
-        <v>0</v>
-      </c>
+      <c r="D29" s="9"/>
       <c r="E29" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7772,11 +7898,11 @@
         <v>78</v>
       </c>
       <c r="D30" s="9">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="E30" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="11">
         <v>0</v>
@@ -7856,11 +7982,11 @@
         <v>0</v>
       </c>
       <c r="AB30" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC30" s="20">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="AD30" s="10">
         <v>0</v>
@@ -8007,11 +8133,11 @@
         <v>80</v>
       </c>
       <c r="D31" s="9">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="E31" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="11">
         <v>0</v>
@@ -8091,11 +8217,11 @@
         <v>0</v>
       </c>
       <c r="AB31" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC31" s="20">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="AD31" s="10">
         <v>0</v>
@@ -8242,11 +8368,11 @@
         <v>81</v>
       </c>
       <c r="D32" s="9">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="E32" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="11">
         <v>0</v>
@@ -8361,11 +8487,11 @@
         <v>0</v>
       </c>
       <c r="AL32" s="10">
-        <v>0</v>
+        <v>0.19</v>
       </c>
       <c r="AM32" s="20">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>15.39</v>
       </c>
       <c r="AN32" s="10">
         <v>0</v>
@@ -8417,11 +8543,11 @@
         <v>0</v>
       </c>
       <c r="BB32" s="10">
-        <v>0</v>
+        <v>0.81</v>
       </c>
       <c r="BC32" s="20">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>65.61</v>
       </c>
       <c r="BD32" s="10">
         <v>0</v>
@@ -8477,11 +8603,11 @@
         <v>82</v>
       </c>
       <c r="D33" s="9">
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="E33" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" s="11">
         <v>0</v>
@@ -8561,11 +8687,11 @@
         <v>0</v>
       </c>
       <c r="AB33" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC33" s="20">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="AD33" s="10">
         <v>0</v>
@@ -8701,7 +8827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>25</v>
       </c>
@@ -8936,7 +9062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>25</v>
       </c>
@@ -9171,7 +9297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>25</v>
       </c>
@@ -9406,7 +9532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>25</v>
       </c>
@@ -9641,7 +9767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>25</v>
       </c>
@@ -9876,7 +10002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>25</v>
       </c>
@@ -10111,7 +10237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>25</v>
       </c>
@@ -10346,7 +10472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>25</v>
       </c>
@@ -10581,7 +10707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>25</v>
       </c>
@@ -10816,7 +10942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>25</v>
       </c>
@@ -11051,7 +11177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>25</v>
       </c>
@@ -11286,7 +11412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>25</v>
       </c>
@@ -11521,7 +11647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>25</v>
       </c>
@@ -11756,7 +11882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>25</v>
       </c>
@@ -11991,7 +12117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>25</v>
       </c>
@@ -12226,7 +12352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>25</v>
       </c>
@@ -12461,7 +12587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>25</v>
       </c>
@@ -12696,7 +12822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>25</v>
       </c>
@@ -12931,7 +13057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>25</v>
       </c>
@@ -13166,7 +13292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -13395,7 +13521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
@@ -13624,7 +13750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
@@ -13853,7 +13979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2"/>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
@@ -14082,7 +14208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -14311,7 +14437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
@@ -14540,7 +14666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
@@ -14769,7 +14895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
@@ -14998,7 +15124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
@@ -15227,7 +15353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -15456,7 +15582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
@@ -15685,7 +15811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2"/>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
@@ -15914,7 +16040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2"/>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
@@ -16143,7 +16269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2"/>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
@@ -16372,7 +16498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2"/>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
@@ -16601,7 +16727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
@@ -16830,7 +16956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
@@ -17059,7 +17185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
@@ -17288,7 +17414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2"/>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
@@ -17517,7 +17643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2"/>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
@@ -17746,7 +17872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
@@ -17975,7 +18101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2"/>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
@@ -18204,7 +18330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2"/>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
@@ -18433,7 +18559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2"/>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
@@ -18662,7 +18788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2"/>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
@@ -18891,7 +19017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2"/>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
@@ -19120,7 +19246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
@@ -19349,7 +19475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
@@ -19578,7 +19704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2"/>
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
@@ -19807,7 +19933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2"/>
       <c r="B82" s="8"/>
       <c r="C82" s="8"/>
@@ -20036,7 +20162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2"/>
       <c r="B83" s="8"/>
       <c r="C83" s="8"/>
@@ -20265,7 +20391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2"/>
       <c r="B84" s="8"/>
       <c r="C84" s="8"/>
@@ -20494,7 +20620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2"/>
       <c r="B85" s="8"/>
       <c r="C85" s="8"/>
@@ -20723,7 +20849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
@@ -20952,7 +21078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="B87" s="8"/>
       <c r="C87" s="8"/>
@@ -21181,7 +21307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
       <c r="B88" s="8"/>
       <c r="C88" s="8"/>
@@ -21410,7 +21536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2"/>
       <c r="B89" s="8"/>
       <c r="C89" s="8"/>
@@ -21639,7 +21765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2"/>
       <c r="B90" s="8"/>
       <c r="C90" s="8"/>
@@ -21868,7 +21994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2"/>
       <c r="B91" s="8"/>
       <c r="C91" s="8"/>
@@ -22097,7 +22223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2"/>
       <c r="B92" s="8"/>
       <c r="C92" s="8"/>
@@ -22326,7 +22452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2"/>
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
@@ -22555,7 +22681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2"/>
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
@@ -22784,7 +22910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2"/>
       <c r="B95" s="8"/>
       <c r="C95" s="8"/>
@@ -23013,7 +23139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2"/>
       <c r="B96" s="8"/>
       <c r="C96" s="8"/>
@@ -23242,7 +23368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2"/>
       <c r="B97" s="8"/>
       <c r="C97" s="8"/>
@@ -23471,7 +23597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2"/>
       <c r="B98" s="8"/>
       <c r="C98" s="8"/>
@@ -23700,7 +23826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2"/>
       <c r="B99" s="8"/>
       <c r="C99" s="8"/>
@@ -23929,7 +24055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2"/>
       <c r="B100" s="8"/>
       <c r="C100" s="8"/>
@@ -24158,7 +24284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2"/>
       <c r="B101" s="8"/>
       <c r="C101" s="8"/>
@@ -24387,7 +24513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2"/>
       <c r="B102" s="8"/>
       <c r="C102" s="8"/>
@@ -24616,7 +24742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2"/>
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
@@ -24845,7 +24971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2"/>
       <c r="B104" s="8"/>
       <c r="C104" s="8"/>
@@ -25074,30 +25200,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:67" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:67" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="14"/>
       <c r="C105" s="14"/>
       <c r="D105" s="15">
         <f>SUM(D3:D104)</f>
-        <v>589775</v>
+        <v>590046</v>
       </c>
       <c r="E105" s="17"/>
       <c r="F105" s="21">
         <f>G105/$D105</f>
-        <v>0</v>
+        <v>3.4743053931388396E-6</v>
       </c>
       <c r="G105" s="22">
         <f>SUM(G3:G104)</f>
-        <v>0</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="H105" s="23">
         <f>I105/$D105</f>
-        <v>0</v>
+        <v>3.8115672337410982E-5</v>
       </c>
       <c r="I105" s="22">
         <f>SUM(I3:I104)</f>
-        <v>0</v>
+        <v>22.490000000000002</v>
       </c>
       <c r="J105" s="23">
         <f>K105/$D105</f>
@@ -25109,19 +25235,19 @@
       </c>
       <c r="L105" s="23">
         <f>M105/$D105</f>
-        <v>0</v>
+        <v>3.779366354487616E-6</v>
       </c>
       <c r="M105" s="22">
         <f>SUM(M3:M104)</f>
-        <v>0</v>
+        <v>2.23</v>
       </c>
       <c r="N105" s="30">
         <f>O105/$D105</f>
-        <v>0</v>
+        <v>8.3951081780064609E-5</v>
       </c>
       <c r="O105" s="31">
         <f>SUM(O3:O104)</f>
-        <v>0</v>
+        <v>49.535000000000004</v>
       </c>
       <c r="P105" s="32">
         <f>Q105/$D105</f>
@@ -25141,19 +25267,19 @@
       </c>
       <c r="T105" s="32">
         <f>U105/$D105</f>
-        <v>3.4361069899537966E-2</v>
+        <v>3.456642363476746E-2</v>
       </c>
       <c r="U105" s="31">
         <f>SUM(U3:U104)</f>
-        <v>20265.300000000003</v>
+        <v>20395.780000000002</v>
       </c>
       <c r="V105" s="32">
         <f>W105/$D105</f>
-        <v>3.1450705777627062E-2</v>
+        <v>3.312934923717812E-2</v>
       </c>
       <c r="W105" s="31">
         <f>SUM(W3:W104)</f>
-        <v>18548.84</v>
+        <v>19547.84</v>
       </c>
       <c r="X105" s="23">
         <f>Y105/$D105</f>
@@ -25165,27 +25291,27 @@
       </c>
       <c r="Z105" s="23">
         <f>AA105/$D105</f>
-        <v>0</v>
+        <v>1.3897221572555358E-5</v>
       </c>
       <c r="AA105" s="22">
         <f>SUM(AA3:AA104)</f>
-        <v>0</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="AB105" s="32">
         <f>AC105/$D105</f>
-        <v>0</v>
+        <v>3.2578815888930691E-4</v>
       </c>
       <c r="AC105" s="31">
         <f>SUM(AC3:AC104)</f>
-        <v>0</v>
+        <v>192.23</v>
       </c>
       <c r="AD105" s="32">
         <f>AE105/$D105</f>
-        <v>0</v>
+        <v>4.6581114014839522E-4</v>
       </c>
       <c r="AE105" s="31">
         <f>SUM(AE3:AE104)</f>
-        <v>0</v>
+        <v>274.85000000000002</v>
       </c>
       <c r="AF105" s="32">
         <f>AG105/$D105</f>
@@ -25197,35 +25323,35 @@
       </c>
       <c r="AH105" s="23">
         <f>AI105/$D105</f>
-        <v>0</v>
+        <v>1.9057836168705491E-5</v>
       </c>
       <c r="AI105" s="22">
         <f>SUM(AI3:AI104)</f>
-        <v>0</v>
+        <v>11.245000000000001</v>
       </c>
       <c r="AJ105" s="32">
         <f>AK105/$D105</f>
-        <v>0</v>
+        <v>1.3611650617070532E-3</v>
       </c>
       <c r="AK105" s="31">
         <f>SUM(AK3:AK104)</f>
-        <v>0</v>
+        <v>803.15</v>
       </c>
       <c r="AL105" s="32">
         <f>AM105/$D105</f>
-        <v>0</v>
+        <v>2.1144961579266702E-4</v>
       </c>
       <c r="AM105" s="31">
         <f>SUM(AM3:AM104)</f>
-        <v>0</v>
+        <v>124.765</v>
       </c>
       <c r="AN105" s="32">
         <f>AO105/$D105</f>
-        <v>3.0601500572252128E-4</v>
+        <v>2.2198777722414863E-3</v>
       </c>
       <c r="AO105" s="31">
         <f>SUM(AO3:AO104)</f>
-        <v>180.48</v>
+        <v>1309.8300000000002</v>
       </c>
       <c r="AP105" s="32">
         <f>AQ105/$D105</f>
@@ -25237,11 +25363,11 @@
       </c>
       <c r="AR105" s="32">
         <f>AS105/$D105</f>
-        <v>0.33248164130388708</v>
+        <v>0.34601244648722301</v>
       </c>
       <c r="AS105" s="31">
         <f>SUM(AS3:AS104)</f>
-        <v>196089.36</v>
+        <v>204163.25999999998</v>
       </c>
       <c r="AT105" s="23">
         <f>AU105/$D105</f>
@@ -25261,11 +25387,11 @@
       </c>
       <c r="AX105" s="23">
         <f>AY105/$D105</f>
-        <v>0</v>
+        <v>7.3706117828101539E-5</v>
       </c>
       <c r="AY105" s="22">
         <f>SUM(AY3:AY104)</f>
-        <v>0</v>
+        <v>43.49</v>
       </c>
       <c r="AZ105" s="23">
         <f>BA105/$D105</f>
@@ -25277,35 +25403,35 @@
       </c>
       <c r="BB105" s="23">
         <f>BC105/$D105</f>
-        <v>0</v>
+        <v>1.6694461109811775E-4</v>
       </c>
       <c r="BC105" s="22">
         <f>SUM(BC3:BC104)</f>
-        <v>0</v>
+        <v>98.504999999999995</v>
       </c>
       <c r="BD105" s="23">
         <f>BE105/$D105</f>
-        <v>0</v>
+        <v>4.9453771400873831E-5</v>
       </c>
       <c r="BE105" s="22">
         <f>SUM(BE3:BE104)</f>
-        <v>0</v>
+        <v>29.18</v>
       </c>
       <c r="BF105" s="32">
         <f>BG105/$D105</f>
-        <v>0</v>
+        <v>2.3621887107106902E-4</v>
       </c>
       <c r="BG105" s="33">
         <f>SUM(BG3:BG104)</f>
-        <v>0</v>
+        <v>139.38</v>
       </c>
       <c r="BH105" s="23">
         <f>BI105/$D105</f>
-        <v>0</v>
+        <v>2.2396558912355986E-5</v>
       </c>
       <c r="BI105" s="22">
         <f>SUM(BI3:BI104)</f>
-        <v>0</v>
+        <v>13.215</v>
       </c>
       <c r="BJ105" s="23">
         <f>BK105/$D105</f>
@@ -25325,7 +25451,7 @@
       </c>
       <c r="BN105" s="27">
         <f>BO105/$D105</f>
-        <v>9.2771005892077499E-2</v>
+        <v>9.2728397446978722E-2</v>
       </c>
       <c r="BO105" s="28">
         <f>SUM(BO3:BO104)</f>
@@ -25334,27 +25460,16 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:BO105" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Lucidian Coast"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A3:BO105">
       <sortCondition ref="B2:B105"/>
     </sortState>
   </autoFilter>
   <mergeCells count="32">
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="AP1:AQ1"/>
-    <mergeCell ref="AT1:AU1"/>
-    <mergeCell ref="AX1:AY1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AR1:AS1"/>
-    <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="BL1:BM1"/>
     <mergeCell ref="BN1:BO1"/>
     <mergeCell ref="X1:Y1"/>
@@ -25371,8 +25486,2623 @@
     <mergeCell ref="AJ1:AK1"/>
     <mergeCell ref="AL1:AM1"/>
     <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AP1:AQ1"/>
+    <mergeCell ref="AT1:AU1"/>
+    <mergeCell ref="AX1:AY1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83BF7E17-4F7C-CF4A-A23F-83F74CCA8F19}">
+  <dimension ref="A1:BM11"/>
+  <sheetViews>
+    <sheetView topLeftCell="N1" zoomScale="234" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1:BK1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="65" width="5.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A1" s="43"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="38"/>
+      <c r="L1" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="36"/>
+      <c r="V1" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="36"/>
+      <c r="AL1" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM1" s="36"/>
+      <c r="AN1" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO1" s="36"/>
+      <c r="AP1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ1" s="36"/>
+      <c r="AR1" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS1" s="38"/>
+      <c r="AT1" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU1" s="38"/>
+      <c r="AV1" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="AW1" s="38"/>
+      <c r="AX1" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="38"/>
+      <c r="AZ1" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="BA1" s="38"/>
+      <c r="BB1" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="BC1" s="38"/>
+      <c r="BD1" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="BE1" s="45"/>
+      <c r="BF1" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="BG1" s="38"/>
+      <c r="BH1" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="BI1" s="38"/>
+      <c r="BJ1" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="BK1" s="38"/>
+      <c r="BL1" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="BM1" s="41"/>
+    </row>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="T2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="U2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="V2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="X2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="AR2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AS2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AW2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="AY2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="BA2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="BC2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="BE2" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="BG2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="BH2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="BI2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="BJ2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL2" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM2" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="9">
+        <v>2230</v>
+      </c>
+      <c r="C3" s="16">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0</v>
+      </c>
+      <c r="E3" s="20">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10">
+        <v>2E-3</v>
+      </c>
+      <c r="G3" s="20">
+        <v>4.46</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0</v>
+      </c>
+      <c r="I3" s="20">
+        <v>0</v>
+      </c>
+      <c r="J3" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="K3" s="20">
+        <v>2.23</v>
+      </c>
+      <c r="L3" s="11">
+        <v>2E-3</v>
+      </c>
+      <c r="M3" s="20">
+        <v>4.46</v>
+      </c>
+      <c r="N3" s="10">
+        <v>0</v>
+      </c>
+      <c r="O3" s="20">
+        <v>0</v>
+      </c>
+      <c r="P3" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="20">
+        <v>0</v>
+      </c>
+      <c r="R3" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="S3" s="20">
+        <v>22.3</v>
+      </c>
+      <c r="T3" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="U3" s="20">
+        <v>89.2</v>
+      </c>
+      <c r="V3" s="10">
+        <v>0</v>
+      </c>
+      <c r="W3" s="20">
+        <v>0</v>
+      </c>
+      <c r="X3" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="AA3" s="20">
+        <v>2.23</v>
+      </c>
+      <c r="AB3" s="10">
+        <v>0.08</v>
+      </c>
+      <c r="AC3" s="20">
+        <v>178.4</v>
+      </c>
+      <c r="AD3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="AG3" s="20">
+        <v>2.23</v>
+      </c>
+      <c r="AH3" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="AI3" s="20">
+        <v>44.6</v>
+      </c>
+      <c r="AJ3" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="AK3" s="20">
+        <v>22.3</v>
+      </c>
+      <c r="AL3" s="10">
+        <v>0.08</v>
+      </c>
+      <c r="AM3" s="20">
+        <v>178.4</v>
+      </c>
+      <c r="AN3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="20">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="10">
+        <v>0.73</v>
+      </c>
+      <c r="AQ3" s="20">
+        <v>1627.8999999999999</v>
+      </c>
+      <c r="AR3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="20">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="10">
+        <v>2E-3</v>
+      </c>
+      <c r="AW3" s="20">
+        <v>4.46</v>
+      </c>
+      <c r="AX3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AY3" s="20">
+        <v>0</v>
+      </c>
+      <c r="AZ3" s="10">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="BA3" s="20">
+        <v>13.38</v>
+      </c>
+      <c r="BB3" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="BC3" s="20">
+        <v>11.15</v>
+      </c>
+      <c r="BD3" s="10">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="BE3" s="20">
+        <v>24.529999999999998</v>
+      </c>
+      <c r="BF3" s="10">
+        <v>0</v>
+      </c>
+      <c r="BG3" s="20">
+        <v>0</v>
+      </c>
+      <c r="BH3" s="10">
+        <v>0</v>
+      </c>
+      <c r="BI3" s="20">
+        <v>0</v>
+      </c>
+      <c r="BJ3" s="10">
+        <v>0</v>
+      </c>
+      <c r="BK3" s="20">
+        <v>0</v>
+      </c>
+      <c r="BL3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM3" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="9">
+        <v>9015</v>
+      </c>
+      <c r="C4" s="16">
+        <v>1</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0</v>
+      </c>
+      <c r="E4" s="20">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10">
+        <v>2E-3</v>
+      </c>
+      <c r="G4" s="20">
+        <v>18.03</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0</v>
+      </c>
+      <c r="I4" s="20">
+        <v>0</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0</v>
+      </c>
+      <c r="K4" s="20">
+        <v>0</v>
+      </c>
+      <c r="L4" s="11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M4" s="20">
+        <v>45.075000000000003</v>
+      </c>
+      <c r="N4" s="10">
+        <v>0</v>
+      </c>
+      <c r="O4" s="20">
+        <v>0</v>
+      </c>
+      <c r="P4" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="20">
+        <v>0</v>
+      </c>
+      <c r="R4" s="10">
+        <v>1.2E-2</v>
+      </c>
+      <c r="S4" s="20">
+        <v>108.18</v>
+      </c>
+      <c r="T4" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="U4" s="20">
+        <v>901.5</v>
+      </c>
+      <c r="V4" s="10">
+        <v>0</v>
+      </c>
+      <c r="W4" s="20">
+        <v>0</v>
+      </c>
+      <c r="X4" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="AC4" s="20">
+        <v>90.15</v>
+      </c>
+      <c r="AD4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="AG4" s="20">
+        <v>9.0150000000000006</v>
+      </c>
+      <c r="AH4" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="AI4" s="20">
+        <v>450.75</v>
+      </c>
+      <c r="AJ4" s="10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AK4" s="20">
+        <v>45.075000000000003</v>
+      </c>
+      <c r="AL4" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="AM4" s="20">
+        <v>901.5</v>
+      </c>
+      <c r="AN4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="AQ4" s="20">
+        <v>6310.5</v>
+      </c>
+      <c r="AR4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="10">
+        <v>2E-3</v>
+      </c>
+      <c r="AW4" s="20">
+        <v>18.03</v>
+      </c>
+      <c r="AX4" s="10">
+        <v>0</v>
+      </c>
+      <c r="AY4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AZ4" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="BA4" s="20">
+        <v>9.0150000000000006</v>
+      </c>
+      <c r="BB4" s="10">
+        <v>2E-3</v>
+      </c>
+      <c r="BC4" s="20">
+        <v>18.03</v>
+      </c>
+      <c r="BD4" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="BE4" s="20">
+        <v>90.15</v>
+      </c>
+      <c r="BF4" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="BG4" s="20">
+        <v>9.0150000000000006</v>
+      </c>
+      <c r="BH4" s="10">
+        <v>0</v>
+      </c>
+      <c r="BI4" s="20">
+        <v>0</v>
+      </c>
+      <c r="BJ4" s="10">
+        <v>0</v>
+      </c>
+      <c r="BK4" s="20">
+        <v>0</v>
+      </c>
+      <c r="BL4" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM4" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="9">
+        <v>410</v>
+      </c>
+      <c r="C5" s="16">
+        <v>1</v>
+      </c>
+      <c r="D5" s="11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E5" s="20">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="F5" s="10">
+        <v>0</v>
+      </c>
+      <c r="G5" s="20">
+        <v>0</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0</v>
+      </c>
+      <c r="I5" s="20">
+        <v>0</v>
+      </c>
+      <c r="J5" s="10">
+        <v>0</v>
+      </c>
+      <c r="K5" s="20">
+        <v>0</v>
+      </c>
+      <c r="L5" s="11">
+        <v>0</v>
+      </c>
+      <c r="M5" s="20">
+        <v>0</v>
+      </c>
+      <c r="N5" s="10">
+        <v>0</v>
+      </c>
+      <c r="O5" s="20">
+        <v>0</v>
+      </c>
+      <c r="P5" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="20">
+        <v>0</v>
+      </c>
+      <c r="R5" s="10">
+        <v>0</v>
+      </c>
+      <c r="S5" s="20">
+        <v>0</v>
+      </c>
+      <c r="T5" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="U5" s="20">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="V5" s="10">
+        <v>0</v>
+      </c>
+      <c r="W5" s="20">
+        <v>0</v>
+      </c>
+      <c r="X5" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="Y5" s="20">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="Z5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="10">
+        <v>0.72</v>
+      </c>
+      <c r="AI5" s="20">
+        <v>295.2</v>
+      </c>
+      <c r="AJ5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="10">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="AM5" s="20">
+        <v>38.950000000000003</v>
+      </c>
+      <c r="AN5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="AQ5" s="20">
+        <v>41</v>
+      </c>
+      <c r="AR5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AU5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AX5" s="10">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="10">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="20">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="10">
+        <v>0</v>
+      </c>
+      <c r="BC5" s="20">
+        <v>0</v>
+      </c>
+      <c r="BD5" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="BE5" s="20">
+        <v>20.5</v>
+      </c>
+      <c r="BF5" s="10">
+        <v>0</v>
+      </c>
+      <c r="BG5" s="20">
+        <v>0</v>
+      </c>
+      <c r="BH5" s="10">
+        <v>0</v>
+      </c>
+      <c r="BI5" s="20">
+        <v>0</v>
+      </c>
+      <c r="BJ5" s="10">
+        <v>0</v>
+      </c>
+      <c r="BK5" s="20">
+        <v>0</v>
+      </c>
+      <c r="BL5" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM5" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="9">
+        <v>210</v>
+      </c>
+      <c r="C6" s="16">
+        <v>1</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0</v>
+      </c>
+      <c r="E6" s="20">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0</v>
+      </c>
+      <c r="G6" s="20">
+        <v>0</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0</v>
+      </c>
+      <c r="I6" s="20">
+        <v>0</v>
+      </c>
+      <c r="J6" s="10">
+        <v>0</v>
+      </c>
+      <c r="K6" s="20">
+        <v>0</v>
+      </c>
+      <c r="L6" s="11">
+        <v>0</v>
+      </c>
+      <c r="M6" s="20">
+        <v>0</v>
+      </c>
+      <c r="N6" s="10">
+        <v>0</v>
+      </c>
+      <c r="O6" s="20">
+        <v>0</v>
+      </c>
+      <c r="P6" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="20">
+        <v>0</v>
+      </c>
+      <c r="R6" s="10">
+        <v>0</v>
+      </c>
+      <c r="S6" s="20">
+        <v>0</v>
+      </c>
+      <c r="T6" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="U6" s="20">
+        <v>4.2</v>
+      </c>
+      <c r="V6" s="10">
+        <v>0</v>
+      </c>
+      <c r="W6" s="20">
+        <v>0</v>
+      </c>
+      <c r="X6" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="AC6" s="20">
+        <v>6.3</v>
+      </c>
+      <c r="AD6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="AI6" s="20">
+        <v>12.6</v>
+      </c>
+      <c r="AJ6" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="AK6" s="20">
+        <v>42</v>
+      </c>
+      <c r="AL6" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="AM6" s="20">
+        <v>10.5</v>
+      </c>
+      <c r="AN6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="10">
+        <v>0.45</v>
+      </c>
+      <c r="AQ6" s="20">
+        <v>94.5</v>
+      </c>
+      <c r="AR6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="AW6" s="20">
+        <v>21</v>
+      </c>
+      <c r="AX6" s="10">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AZ6" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="BA6" s="20">
+        <v>10.5</v>
+      </c>
+      <c r="BB6" s="10">
+        <v>0</v>
+      </c>
+      <c r="BC6" s="20">
+        <v>0</v>
+      </c>
+      <c r="BD6" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BE6" s="20">
+        <v>4.2</v>
+      </c>
+      <c r="BF6" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="BG6" s="20">
+        <v>4.2</v>
+      </c>
+      <c r="BH6" s="10">
+        <v>0</v>
+      </c>
+      <c r="BI6" s="20">
+        <v>0</v>
+      </c>
+      <c r="BJ6" s="10">
+        <v>0</v>
+      </c>
+      <c r="BK6" s="20">
+        <v>0</v>
+      </c>
+      <c r="BL6" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM6" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="16">
+        <v>0</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0</v>
+      </c>
+      <c r="E7" s="20">
+        <v>0</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0</v>
+      </c>
+      <c r="G7" s="20">
+        <v>0</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0</v>
+      </c>
+      <c r="I7" s="20">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10">
+        <v>0</v>
+      </c>
+      <c r="K7" s="20">
+        <v>0</v>
+      </c>
+      <c r="L7" s="11">
+        <v>0</v>
+      </c>
+      <c r="M7" s="20">
+        <v>0</v>
+      </c>
+      <c r="N7" s="10">
+        <v>0</v>
+      </c>
+      <c r="O7" s="20">
+        <v>0</v>
+      </c>
+      <c r="P7" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="20">
+        <v>0</v>
+      </c>
+      <c r="R7" s="10">
+        <v>0</v>
+      </c>
+      <c r="S7" s="20">
+        <v>0</v>
+      </c>
+      <c r="T7" s="10">
+        <v>0</v>
+      </c>
+      <c r="U7" s="20">
+        <v>0</v>
+      </c>
+      <c r="V7" s="10">
+        <v>0</v>
+      </c>
+      <c r="W7" s="20">
+        <v>0</v>
+      </c>
+      <c r="X7" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AW7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AX7" s="10">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AZ7" s="10">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="20">
+        <v>0</v>
+      </c>
+      <c r="BB7" s="10">
+        <v>0</v>
+      </c>
+      <c r="BC7" s="20">
+        <v>0</v>
+      </c>
+      <c r="BD7" s="10">
+        <v>0</v>
+      </c>
+      <c r="BE7" s="20">
+        <v>0</v>
+      </c>
+      <c r="BF7" s="10">
+        <v>0</v>
+      </c>
+      <c r="BG7" s="20">
+        <v>0</v>
+      </c>
+      <c r="BH7" s="10">
+        <v>0</v>
+      </c>
+      <c r="BI7" s="20">
+        <v>0</v>
+      </c>
+      <c r="BJ7" s="10">
+        <v>0</v>
+      </c>
+      <c r="BK7" s="20">
+        <v>0</v>
+      </c>
+      <c r="BL7" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM7" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="9">
+        <v>42</v>
+      </c>
+      <c r="C8" s="16">
+        <v>1</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0</v>
+      </c>
+      <c r="E8" s="20">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="20">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0</v>
+      </c>
+      <c r="I8" s="20">
+        <v>0</v>
+      </c>
+      <c r="J8" s="10">
+        <v>0</v>
+      </c>
+      <c r="K8" s="20">
+        <v>0</v>
+      </c>
+      <c r="L8" s="11">
+        <v>0</v>
+      </c>
+      <c r="M8" s="20">
+        <v>0</v>
+      </c>
+      <c r="N8" s="10">
+        <v>0</v>
+      </c>
+      <c r="O8" s="20">
+        <v>0</v>
+      </c>
+      <c r="P8" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="20">
+        <v>0</v>
+      </c>
+      <c r="R8" s="10">
+        <v>0</v>
+      </c>
+      <c r="S8" s="20">
+        <v>0</v>
+      </c>
+      <c r="T8" s="10">
+        <v>0</v>
+      </c>
+      <c r="U8" s="20">
+        <v>0</v>
+      </c>
+      <c r="V8" s="10">
+        <v>0</v>
+      </c>
+      <c r="W8" s="20">
+        <v>0</v>
+      </c>
+      <c r="X8" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="10">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="20">
+        <v>42</v>
+      </c>
+      <c r="AB8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AW8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AX8" s="10">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AZ8" s="10">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="20">
+        <v>0</v>
+      </c>
+      <c r="BB8" s="10">
+        <v>0</v>
+      </c>
+      <c r="BC8" s="20">
+        <v>0</v>
+      </c>
+      <c r="BD8" s="10">
+        <v>0</v>
+      </c>
+      <c r="BE8" s="20">
+        <v>0</v>
+      </c>
+      <c r="BF8" s="10">
+        <v>0</v>
+      </c>
+      <c r="BG8" s="20">
+        <v>0</v>
+      </c>
+      <c r="BH8" s="10">
+        <v>0</v>
+      </c>
+      <c r="BI8" s="20">
+        <v>0</v>
+      </c>
+      <c r="BJ8" s="10">
+        <v>0</v>
+      </c>
+      <c r="BK8" s="20">
+        <v>0</v>
+      </c>
+      <c r="BL8" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM8" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="9">
+        <v>36</v>
+      </c>
+      <c r="C9" s="16">
+        <v>1</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
+      <c r="E9" s="20">
+        <v>0</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0</v>
+      </c>
+      <c r="G9" s="20">
+        <v>0</v>
+      </c>
+      <c r="H9" s="10">
+        <v>0</v>
+      </c>
+      <c r="I9" s="20">
+        <v>0</v>
+      </c>
+      <c r="J9" s="10">
+        <v>0</v>
+      </c>
+      <c r="K9" s="20">
+        <v>0</v>
+      </c>
+      <c r="L9" s="11">
+        <v>0</v>
+      </c>
+      <c r="M9" s="20">
+        <v>0</v>
+      </c>
+      <c r="N9" s="10">
+        <v>0</v>
+      </c>
+      <c r="O9" s="20">
+        <v>0</v>
+      </c>
+      <c r="P9" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="20">
+        <v>0</v>
+      </c>
+      <c r="R9" s="10">
+        <v>0</v>
+      </c>
+      <c r="S9" s="20">
+        <v>0</v>
+      </c>
+      <c r="T9" s="10">
+        <v>0</v>
+      </c>
+      <c r="U9" s="20">
+        <v>0</v>
+      </c>
+      <c r="V9" s="10">
+        <v>0</v>
+      </c>
+      <c r="W9" s="20">
+        <v>0</v>
+      </c>
+      <c r="X9" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="10">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="20">
+        <v>36</v>
+      </c>
+      <c r="AB9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AX9" s="10">
+        <v>0</v>
+      </c>
+      <c r="AY9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AZ9" s="10">
+        <v>0</v>
+      </c>
+      <c r="BA9" s="20">
+        <v>0</v>
+      </c>
+      <c r="BB9" s="10">
+        <v>0</v>
+      </c>
+      <c r="BC9" s="20">
+        <v>0</v>
+      </c>
+      <c r="BD9" s="10">
+        <v>0</v>
+      </c>
+      <c r="BE9" s="20">
+        <v>0</v>
+      </c>
+      <c r="BF9" s="10">
+        <v>0</v>
+      </c>
+      <c r="BG9" s="20">
+        <v>0</v>
+      </c>
+      <c r="BH9" s="10">
+        <v>0</v>
+      </c>
+      <c r="BI9" s="20">
+        <v>0</v>
+      </c>
+      <c r="BJ9" s="10">
+        <v>0</v>
+      </c>
+      <c r="BK9" s="20">
+        <v>0</v>
+      </c>
+      <c r="BL9" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM9" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="9">
+        <v>81</v>
+      </c>
+      <c r="C10" s="16">
+        <v>1</v>
+      </c>
+      <c r="D10" s="11">
+        <v>0</v>
+      </c>
+      <c r="E10" s="20">
+        <v>0</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="20">
+        <v>0</v>
+      </c>
+      <c r="H10" s="10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="20">
+        <v>0</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0</v>
+      </c>
+      <c r="K10" s="20">
+        <v>0</v>
+      </c>
+      <c r="L10" s="11">
+        <v>0</v>
+      </c>
+      <c r="M10" s="20">
+        <v>0</v>
+      </c>
+      <c r="N10" s="10">
+        <v>0</v>
+      </c>
+      <c r="O10" s="20">
+        <v>0</v>
+      </c>
+      <c r="P10" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="20">
+        <v>0</v>
+      </c>
+      <c r="R10" s="10">
+        <v>0</v>
+      </c>
+      <c r="S10" s="20">
+        <v>0</v>
+      </c>
+      <c r="T10" s="10">
+        <v>0</v>
+      </c>
+      <c r="U10" s="20">
+        <v>0</v>
+      </c>
+      <c r="V10" s="10">
+        <v>0</v>
+      </c>
+      <c r="W10" s="20">
+        <v>0</v>
+      </c>
+      <c r="X10" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="20">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="20">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="20">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="10">
+        <v>0.19</v>
+      </c>
+      <c r="AK10" s="20">
+        <v>15.39</v>
+      </c>
+      <c r="AL10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AM10" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO10" s="20">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="20">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS10" s="20">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AU10" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AW10" s="20">
+        <v>0</v>
+      </c>
+      <c r="AX10" s="10">
+        <v>0</v>
+      </c>
+      <c r="AY10" s="20">
+        <v>0</v>
+      </c>
+      <c r="AZ10" s="10">
+        <v>0.81</v>
+      </c>
+      <c r="BA10" s="20">
+        <v>65.61</v>
+      </c>
+      <c r="BB10" s="10">
+        <v>0</v>
+      </c>
+      <c r="BC10" s="20">
+        <v>0</v>
+      </c>
+      <c r="BD10" s="10">
+        <v>0</v>
+      </c>
+      <c r="BE10" s="20">
+        <v>0</v>
+      </c>
+      <c r="BF10" s="10">
+        <v>0</v>
+      </c>
+      <c r="BG10" s="20">
+        <v>0</v>
+      </c>
+      <c r="BH10" s="10">
+        <v>0</v>
+      </c>
+      <c r="BI10" s="20">
+        <v>0</v>
+      </c>
+      <c r="BJ10" s="10">
+        <v>0</v>
+      </c>
+      <c r="BK10" s="20">
+        <v>0</v>
+      </c>
+      <c r="BL10" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM10" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="9">
+        <v>112</v>
+      </c>
+      <c r="C11" s="16">
+        <v>1</v>
+      </c>
+      <c r="D11" s="11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="20">
+        <v>0</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0</v>
+      </c>
+      <c r="G11" s="20">
+        <v>0</v>
+      </c>
+      <c r="H11" s="10">
+        <v>0</v>
+      </c>
+      <c r="I11" s="20">
+        <v>0</v>
+      </c>
+      <c r="J11" s="10">
+        <v>0</v>
+      </c>
+      <c r="K11" s="20">
+        <v>0</v>
+      </c>
+      <c r="L11" s="11">
+        <v>0</v>
+      </c>
+      <c r="M11" s="20">
+        <v>0</v>
+      </c>
+      <c r="N11" s="10">
+        <v>0</v>
+      </c>
+      <c r="O11" s="20">
+        <v>0</v>
+      </c>
+      <c r="P11" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="20">
+        <v>0</v>
+      </c>
+      <c r="R11" s="10">
+        <v>0</v>
+      </c>
+      <c r="S11" s="20">
+        <v>0</v>
+      </c>
+      <c r="T11" s="10">
+        <v>0</v>
+      </c>
+      <c r="U11" s="20">
+        <v>0</v>
+      </c>
+      <c r="V11" s="10">
+        <v>0</v>
+      </c>
+      <c r="W11" s="20">
+        <v>0</v>
+      </c>
+      <c r="X11" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="10">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="20">
+        <v>112</v>
+      </c>
+      <c r="AB11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="20">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="20">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AM11" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO11" s="20">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="20">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AS11" s="20">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AU11" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AW11" s="20">
+        <v>0</v>
+      </c>
+      <c r="AX11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AY11" s="20">
+        <v>0</v>
+      </c>
+      <c r="AZ11" s="10">
+        <v>0</v>
+      </c>
+      <c r="BA11" s="20">
+        <v>0</v>
+      </c>
+      <c r="BB11" s="10">
+        <v>0</v>
+      </c>
+      <c r="BC11" s="20">
+        <v>0</v>
+      </c>
+      <c r="BD11" s="10">
+        <v>0</v>
+      </c>
+      <c r="BE11" s="20">
+        <v>0</v>
+      </c>
+      <c r="BF11" s="10">
+        <v>0</v>
+      </c>
+      <c r="BG11" s="20">
+        <v>0</v>
+      </c>
+      <c r="BH11" s="10">
+        <v>0</v>
+      </c>
+      <c r="BI11" s="20">
+        <v>0</v>
+      </c>
+      <c r="BJ11" s="10">
+        <v>0</v>
+      </c>
+      <c r="BK11" s="20">
+        <v>0</v>
+      </c>
+      <c r="BL11" s="5">
+        <v>0</v>
+      </c>
+      <c r="BM11" s="26">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="32">
+    <mergeCell ref="BJ1:BK1"/>
+    <mergeCell ref="BL1:BM1"/>
+    <mergeCell ref="AX1:AY1"/>
+    <mergeCell ref="AZ1:BA1"/>
+    <mergeCell ref="BB1:BC1"/>
+    <mergeCell ref="BD1:BE1"/>
+    <mergeCell ref="BF1:BG1"/>
+    <mergeCell ref="BH1:BI1"/>
+    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AP1:AQ1"/>
+    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="AT1:AU1"/>
+    <mergeCell ref="AV1:AW1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDDAB8B2-70BE-D844-8241-0961C8E855CE}">
+  <dimension ref="A1:E38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="288" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19:E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="53"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="54" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="56"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="55">
+        <f>(SUM(D5:D17))</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="52"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="51">
+        <v>0</v>
+      </c>
+      <c r="E5" s="50">
+        <f>E$3*D5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="52"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="51">
+        <v>0</v>
+      </c>
+      <c r="E6" s="50">
+        <f>E$3*D6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="52"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="51">
+        <v>0</v>
+      </c>
+      <c r="E7" s="50">
+        <f>E$3*D7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="52"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="51">
+        <v>0</v>
+      </c>
+      <c r="E8" s="50">
+        <f>E$3*D8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="52"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="51">
+        <v>0</v>
+      </c>
+      <c r="E9" s="50">
+        <f>E$3*D9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="52"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="51">
+        <v>0</v>
+      </c>
+      <c r="E10" s="50">
+        <f>E$3*D10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="52"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="51">
+        <v>0</v>
+      </c>
+      <c r="E11" s="50">
+        <f>E$3*D11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="52"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="51">
+        <v>0</v>
+      </c>
+      <c r="E12" s="50">
+        <f>E$3*D12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="52"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="51">
+        <v>0</v>
+      </c>
+      <c r="E13" s="50">
+        <f>E$3*D13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="52"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="51">
+        <v>0</v>
+      </c>
+      <c r="E14" s="50">
+        <f>E$3*D14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="52"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51">
+        <v>0</v>
+      </c>
+      <c r="E15" s="50">
+        <f>E$3*D15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="52"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51">
+        <v>0</v>
+      </c>
+      <c r="E16" s="50">
+        <f>E$3*D16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="59"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="51">
+        <v>0</v>
+      </c>
+      <c r="E17" s="60">
+        <f>E$3*D17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="61" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="62"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="65"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="66"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="65"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="66"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="65"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="66"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="65"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="66"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="65"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="66"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="64" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="65"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="66"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="64" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="65"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="66"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="65"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="66"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="65"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="66"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="65"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="66"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="65"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="66"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="65"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="66"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="65"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="66"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="65"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="66"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="65"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="66"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="65"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="66"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="65"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="66"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="65"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="66"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="65"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="66"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="65"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="66"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
AS region page done.
</commit_message>
<xml_diff>
--- a/development/tools/PopulationCalculator.xlsx
+++ b/development/tools/PopulationCalculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/Documents/GitHub/Atlas-Exandria/development/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC8A595-BBE0-2846-AD82-F5FE7BC82595}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED63B01E-F90A-9642-A85B-055EB9D13A3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" tabRatio="918" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="1280" windowWidth="49540" windowHeight="27700" tabRatio="918" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population" sheetId="14" r:id="rId1"/>
@@ -812,7 +812,16 @@
     <xf numFmtId="10" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="9" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -821,13 +830,10 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -842,13 +848,7 @@
     <xf numFmtId="1" fontId="1" fillId="9" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1137,7 +1137,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J55" sqref="J55"/>
+      <selection pane="bottomLeft" activeCell="AF6" sqref="AF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -1158,9 +1158,9 @@
     <col min="15" max="15" width="9.1640625" style="32" customWidth="1"/>
     <col min="16" max="16" width="9.1640625" style="36" customWidth="1"/>
     <col min="17" max="17" width="9.1640625" style="32" customWidth="1"/>
-    <col min="18" max="18" width="9.1640625" style="36" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="9.1640625" style="32" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="9.1640625" style="40" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9.1640625" style="36" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="9.1640625" style="32" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="20" width="9.1640625" style="40" customWidth="1"/>
     <col min="21" max="21" width="9.1640625" style="32" customWidth="1"/>
     <col min="22" max="22" width="9.1640625" style="36" customWidth="1"/>
     <col min="23" max="23" width="9.1640625" style="32" customWidth="1"/>
@@ -1213,136 +1213,136 @@
       <c r="A1" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="55">
+      <c r="B1" s="45">
         <f>SUM(B51,B2)</f>
         <v>2524854</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="49">
+      <c r="C1" s="46"/>
+      <c r="D1" s="52">
         <f>SUM(D2,D51)</f>
         <v>406067.39999999997</v>
       </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="45" t="s">
+      <c r="E1" s="46"/>
+      <c r="F1" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45" t="s">
+      <c r="G1" s="51"/>
+      <c r="H1" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45" t="s">
+      <c r="I1" s="51"/>
+      <c r="J1" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45" t="s">
+      <c r="K1" s="51"/>
+      <c r="L1" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="45"/>
-      <c r="N1" s="46" t="s">
+      <c r="M1" s="51"/>
+      <c r="N1" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="47"/>
-      <c r="P1" s="46" t="s">
+      <c r="O1" s="50"/>
+      <c r="P1" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="56" t="s">
+      <c r="Q1" s="50"/>
+      <c r="R1" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="S1" s="57"/>
-      <c r="T1" s="46" t="s">
+      <c r="S1" s="48"/>
+      <c r="T1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="U1" s="47"/>
-      <c r="V1" s="46" t="s">
+      <c r="U1" s="50"/>
+      <c r="V1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="47"/>
-      <c r="X1" s="45" t="s">
+      <c r="W1" s="50"/>
+      <c r="X1" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45" t="s">
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" s="45"/>
-      <c r="AB1" s="45" t="s">
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="AC1" s="45"/>
-      <c r="AD1" s="46" t="s">
+      <c r="AC1" s="51"/>
+      <c r="AD1" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="AE1" s="47"/>
-      <c r="AF1" s="45" t="s">
+      <c r="AE1" s="50"/>
+      <c r="AF1" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="45"/>
-      <c r="AH1" s="56" t="s">
+      <c r="AG1" s="51"/>
+      <c r="AH1" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="AI1" s="57"/>
-      <c r="AJ1" s="46" t="s">
+      <c r="AI1" s="48"/>
+      <c r="AJ1" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="AK1" s="47"/>
-      <c r="AL1" s="46" t="s">
+      <c r="AK1" s="50"/>
+      <c r="AL1" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="AM1" s="47"/>
-      <c r="AN1" s="46" t="s">
+      <c r="AM1" s="50"/>
+      <c r="AN1" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="AO1" s="47"/>
-      <c r="AP1" s="48" t="s">
+      <c r="AO1" s="50"/>
+      <c r="AP1" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="AQ1" s="48"/>
-      <c r="AR1" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="AS1" s="47"/>
-      <c r="AT1" s="45" t="s">
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS1" s="50"/>
+      <c r="AT1" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="AU1" s="45"/>
-      <c r="AV1" s="45" t="s">
+      <c r="AU1" s="51"/>
+      <c r="AV1" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="AW1" s="45"/>
-      <c r="AX1" s="45" t="s">
+      <c r="AW1" s="51"/>
+      <c r="AX1" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="AY1" s="45"/>
-      <c r="AZ1" s="45" t="s">
+      <c r="AY1" s="51"/>
+      <c r="AZ1" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="BA1" s="45"/>
-      <c r="BB1" s="45" t="s">
+      <c r="BA1" s="51"/>
+      <c r="BB1" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="BC1" s="45"/>
-      <c r="BD1" s="45" t="s">
+      <c r="BC1" s="51"/>
+      <c r="BD1" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="BE1" s="45"/>
-      <c r="BF1" s="46" t="s">
+      <c r="BE1" s="51"/>
+      <c r="BF1" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="BG1" s="47"/>
-      <c r="BH1" s="45" t="s">
+      <c r="BG1" s="50"/>
+      <c r="BH1" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="BI1" s="45"/>
-      <c r="BJ1" s="45" t="s">
+      <c r="BI1" s="51"/>
+      <c r="BJ1" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="BK1" s="45"/>
-      <c r="BL1" s="45" t="s">
+      <c r="BK1" s="51"/>
+      <c r="BL1" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="BM1" s="45"/>
+      <c r="BM1" s="51"/>
     </row>
     <row r="2" spans="1:65" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -1354,13 +1354,13 @@
       </c>
       <c r="C2" s="41">
         <f>IFERROR(SUM(F2,H2,J2,L2,N2,P2,R2,T2,V2,X2,Z2,AB2,AD2,AF2,AH2,AJ2,AL2,AN2,AP2,AR2,AT2,AV2,AX2,AZ2,BB2,BD2,BF2,BH2,BJ2,BL2),0)</f>
-        <v>1</v>
-      </c>
-      <c r="D2" s="51">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="D2" s="53">
         <f>SUM(E46,E42,E33,E27,E22,E13,E6,E3)</f>
         <v>406067.39999999997</v>
       </c>
-      <c r="E2" s="52">
+      <c r="E2" s="54">
         <f>SUM(E46,E42,E33,E27,E22,E13,E6,E3)</f>
         <v>406067.39999999997</v>
       </c>
@@ -1382,27 +1382,27 @@
       </c>
       <c r="J2" s="34">
         <f>IFERROR(K2/$B2,0)</f>
-        <v>1.2509214548289311E-2</v>
+        <v>1.2529885615535731E-2</v>
       </c>
       <c r="K2" s="31">
         <f>SUM(K46,K42,K33,K27,K22,K13,K6,K3)</f>
-        <v>12805.094999999998</v>
+        <v>12826.254999999997</v>
       </c>
       <c r="L2" s="34">
         <f>IFERROR(M2/$B2,0)</f>
-        <v>1.4030745770295208E-3</v>
+        <v>1.413410110652731E-3</v>
       </c>
       <c r="M2" s="31">
         <f>SUM(M46,M42,M33,M27,M22,M13,M6,M3)</f>
-        <v>1436.2615000000001</v>
+        <v>1446.8415</v>
       </c>
       <c r="N2" s="37">
         <f>IFERROR(O2/$B2,0)</f>
-        <v>3.6481717925898717E-3</v>
+        <v>3.6471382392275508E-3</v>
       </c>
       <c r="O2" s="33">
         <f>SUM(O46,O42,O33,O27,O22,O13,O6,O3)</f>
-        <v>3734.462</v>
+        <v>3733.404</v>
       </c>
       <c r="P2" s="37">
         <f>IFERROR(Q2/$B2,0)</f>
@@ -1422,19 +1422,19 @@
       </c>
       <c r="T2" s="38">
         <f>IFERROR(U2/$B2,0)</f>
-        <v>9.9960746463889624E-2</v>
+        <v>9.997108199751284E-2</v>
       </c>
       <c r="U2" s="33">
         <f>SUM(U46,U42,U33,U27,U22,U13,U6,U3)</f>
-        <v>102325.118</v>
+        <v>102335.698</v>
       </c>
       <c r="V2" s="37">
         <f>IFERROR(W2/$B2,0)</f>
-        <v>9.7512107130052872E-2</v>
+        <v>9.7557571755272549E-2</v>
       </c>
       <c r="W2" s="33">
         <f>SUM(W46,W42,W33,W27,W22,W13,W6,W3)</f>
-        <v>99818.561000000016</v>
+        <v>99865.10100000001</v>
       </c>
       <c r="X2" s="34">
         <f>IFERROR(Y2/$B2,0)</f>
@@ -1454,75 +1454,75 @@
       </c>
       <c r="AB2" s="34">
         <f>IFERROR(AC2/$B2,0)</f>
-        <v>3.4031791046379972E-3</v>
+        <v>3.4610580929279743E-3</v>
       </c>
       <c r="AC2" s="31">
         <f>SUM(AC46,AC42,AC33,AC27,AC22,AC13,AC6,AC3)</f>
-        <v>3483.6744999999996</v>
+        <v>3542.9224999999997</v>
       </c>
       <c r="AD2" s="37">
         <f>IFERROR(AE2/$B2,0)</f>
-        <v>3.6996879802042297E-2</v>
+        <v>3.699998046212926E-2</v>
       </c>
       <c r="AE2" s="33">
         <f>SUM(AE46,AE42,AE33,AE27,AE22,AE13,AE6,AE3)</f>
-        <v>37871.967000000004</v>
+        <v>37875.141000000003</v>
       </c>
       <c r="AF2" s="34">
         <f>IFERROR(AG2/$B2,0)</f>
-        <v>3.4131947056277867E-2</v>
+        <v>3.411127598903145E-2</v>
       </c>
       <c r="AG2" s="31">
         <f>SUM(AG46,AG42,AG33,AG27,AG22,AG13,AG6,AG3)</f>
-        <v>34939.270000000004</v>
+        <v>34918.110000000008</v>
       </c>
       <c r="AH2" s="34">
         <f>IFERROR(AI2/$B2,0)</f>
-        <v>2.7865541350438087E-3</v>
+        <v>2.7555475341741781E-3</v>
       </c>
       <c r="AI2" s="31">
         <f>SUM(AI46,AI42,AI33,AI27,AI22,AI13,AI6,AI3)</f>
-        <v>2852.4645</v>
+        <v>2820.7244999999998</v>
       </c>
       <c r="AJ2" s="37">
         <f>IFERROR(AK2/$B2,0)</f>
-        <v>4.8106498979634697E-2</v>
+        <v>4.8082737021236686E-2</v>
       </c>
       <c r="AK2" s="33">
         <f>SUM(AK46,AK42,AK33,AK27,AK22,AK13,AK6,AK3)</f>
-        <v>49244.361999999994</v>
+        <v>49220.038</v>
       </c>
       <c r="AL2" s="37">
         <f>IFERROR(AM2/$B2,0)</f>
-        <v>3.0348485766172714E-2</v>
+        <v>3.0334017972887296E-2</v>
       </c>
       <c r="AM2" s="33">
         <f>SUM(AM46,AM42,AM33,AM27,AM22,AM13,AM6,AM3)</f>
-        <v>31066.318499999998</v>
+        <v>31051.5085</v>
       </c>
       <c r="AN2" s="37">
         <f>IFERROR(AO2/$B2,0)</f>
-        <v>5.2806541865260986E-2</v>
+        <v>5.2801374098449379E-2</v>
       </c>
       <c r="AO2" s="33">
         <f>SUM(AO46,AO42,AO33,AO27,AO22,AO13,AO6,AO3)</f>
-        <v>54055.575000000004</v>
+        <v>54050.285000000003</v>
       </c>
       <c r="AP2" s="37">
         <f>IFERROR(AQ2/$B2,0)</f>
-        <v>0.11310983800174473</v>
+        <v>0.11316151566986078</v>
       </c>
       <c r="AQ2" s="33">
         <f>SUM(AQ46,AQ42,AQ33,AQ27,AQ22,AQ13,AQ6,AQ3)</f>
-        <v>115785.22500000001</v>
+        <v>115838.125</v>
       </c>
       <c r="AR2" s="37">
         <f>IFERROR(AS2/$B2,0)</f>
-        <v>0.36605247579013594</v>
+        <v>0.36582509405042529</v>
       </c>
       <c r="AS2" s="33">
         <f>SUM(AS46,AS42,AS33,AS27,AS22,AS13,AS6,AS3)</f>
-        <v>374710.71500000003</v>
+        <v>374477.95500000002</v>
       </c>
       <c r="AT2" s="34">
         <f>IFERROR(AU2/$B2,0)</f>
@@ -1534,19 +1534,19 @@
       </c>
       <c r="AV2" s="34">
         <f>IFERROR(AW2/$B2,0)</f>
-        <v>6.2470143691270375E-3</v>
+        <v>6.2676854363734585E-3</v>
       </c>
       <c r="AW2" s="31">
         <f>SUM(AW46,AW42,AW33,AW27,AW22,AW13,AW6,AW3)</f>
-        <v>6394.7749999999996</v>
+        <v>6415.9349999999995</v>
       </c>
       <c r="AX2" s="34">
         <f>IFERROR(AY2/$B2,0)</f>
-        <v>7.3210497111814267E-3</v>
+        <v>7.3520563120510569E-3</v>
       </c>
       <c r="AY2" s="31">
         <f>SUM(AY46,AY42,AY33,AY27,AY22,AY13,AY6,AY3)</f>
-        <v>7494.214500000001</v>
+        <v>7525.9545000000007</v>
       </c>
       <c r="AZ2" s="34">
         <f>IFERROR(BA2/$B2,0)</f>
@@ -1558,11 +1558,11 @@
       </c>
       <c r="BB2" s="34">
         <f>IFERROR(BC2/$B2,0)</f>
-        <v>1.4371987382443073E-2</v>
+        <v>1.4444336117805547E-2</v>
       </c>
       <c r="BC2" s="31">
         <f>SUM(BC46,BC42,BC33,BC27,BC22,BC13,BC6,BC3)</f>
-        <v>14711.928</v>
+        <v>14785.988000000001</v>
       </c>
       <c r="BD2" s="34">
         <f>IFERROR(BE2/$B2,0)</f>
@@ -1615,7 +1615,7 @@
       </c>
       <c r="C3" s="42">
         <f>IFERROR(SUM(F3,H3,J3,L3,N3,P3,R3,T3,V3,X3,Z3,AB3,AD3,AF3,AH3,AJ3,AL3,AN3,AP3,AR3,AT3,AV3,AX3,AZ3,BB3,BD3,BF3,BH3,BJ3,BL3),0)</f>
-        <v>0.99999999999999978</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="D3" s="28">
         <v>84</v>
@@ -1642,27 +1642,27 @@
       </c>
       <c r="J3" s="34">
         <f>IFERROR(K3/$B3,0)</f>
-        <v>2.0007564296520425E-3</v>
+        <v>6.0022692889561266E-3</v>
       </c>
       <c r="K3" s="31">
         <f>SUM(K4:K5)</f>
-        <v>10.58</v>
+        <v>31.74</v>
       </c>
       <c r="L3" s="34">
         <f>IFERROR(M3/$B3,0)</f>
-        <v>1.4805219364599094E-2</v>
+        <v>1.6805975794251134E-2</v>
       </c>
       <c r="M3" s="31">
         <f>SUM(M4:M5)</f>
-        <v>78.290000000000006</v>
+        <v>88.87</v>
       </c>
       <c r="N3" s="37">
         <f>IFERROR(O3/$B3,0)</f>
-        <v>2.7999243570347955E-3</v>
+        <v>2.5998487140695913E-3</v>
       </c>
       <c r="O3" s="33">
         <f>SUM(O4:O5)</f>
-        <v>14.805999999999999</v>
+        <v>13.747999999999999</v>
       </c>
       <c r="P3" s="37">
         <f>IFERROR(Q3/$B3,0)</f>
@@ -1682,19 +1682,19 @@
       </c>
       <c r="T3" s="38">
         <f>IFERROR(U3/$B3,0)</f>
-        <v>5.7999243570347955E-2</v>
+        <v>0.06</v>
       </c>
       <c r="U3" s="33">
         <f>SUM(U4:U5)</f>
-        <v>306.7</v>
+        <v>317.27999999999997</v>
       </c>
       <c r="V3" s="37">
         <f>IFERROR(W3/$B3,0)</f>
-        <v>5.0000000000000001E-3</v>
+        <v>1.3801059001512857E-2</v>
       </c>
       <c r="W3" s="33">
         <f>SUM(W4:W5)</f>
-        <v>26.44</v>
+        <v>72.97999999999999</v>
       </c>
       <c r="X3" s="34">
         <f>IFERROR(Y3/$B3,0)</f>
@@ -1714,75 +1714,75 @@
       </c>
       <c r="AB3" s="34">
         <f>IFERROR(AC3/$B3,0)</f>
-        <v>1.4805597579425114E-2</v>
+        <v>2.6009833585476549E-2</v>
       </c>
       <c r="AC3" s="31">
         <f>SUM(AC4:AC5)</f>
-        <v>78.292000000000002</v>
+        <v>137.54</v>
       </c>
       <c r="AD3" s="37">
         <f>IFERROR(AE3/$B3,0)</f>
-        <v>4.3997730711043881E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AE3" s="33">
         <f>SUM(AE4:AE5)</f>
-        <v>23.266000000000002</v>
+        <v>26.44</v>
       </c>
       <c r="AF3" s="34">
         <f>IFERROR(AG3/$B3,0)</f>
-        <v>4.001512859304085E-2</v>
+        <v>3.6013615733736765E-2</v>
       </c>
       <c r="AG3" s="31">
         <f>SUM(AG4:AG5)</f>
-        <v>211.60000000000002</v>
+        <v>190.44</v>
       </c>
       <c r="AH3" s="34">
         <f>IFERROR(AI3/$B3,0)</f>
-        <v>1.0803706505295009E-2</v>
+        <v>4.8014372163388804E-3</v>
       </c>
       <c r="AI3" s="31">
         <f>SUM(AI4:AI5)</f>
-        <v>57.13000000000001</v>
+        <v>25.39</v>
       </c>
       <c r="AJ3" s="37">
         <f>IFERROR(AK3/$B3,0)</f>
-        <v>8.999621785173979E-3</v>
+        <v>4.3997730711043881E-3</v>
       </c>
       <c r="AK3" s="33">
         <f>SUM(AK4:AK5)</f>
-        <v>47.59</v>
+        <v>23.266000000000002</v>
       </c>
       <c r="AL3" s="37">
         <f>IFERROR(AM3/$B3,0)</f>
-        <v>5.6013615733736767E-3</v>
+        <v>2.8006807866868383E-3</v>
       </c>
       <c r="AM3" s="33">
         <f>SUM(AM4:AM5)</f>
-        <v>29.62</v>
+        <v>14.81</v>
       </c>
       <c r="AN3" s="37">
         <f>IFERROR(AO3/$B3,0)</f>
-        <v>5.9996217851739794E-2</v>
+        <v>5.8995839636913773E-2</v>
       </c>
       <c r="AO3" s="33">
         <f>SUM(AO4:AO5)</f>
-        <v>317.26000000000005</v>
+        <v>311.97000000000003</v>
       </c>
       <c r="AP3" s="37">
         <f>IFERROR(AQ3/$B3,0)</f>
-        <v>0</v>
+        <v>1.0003782148260212E-2</v>
       </c>
       <c r="AQ3" s="33">
         <f>SUM(AQ4:AQ5)</f>
-        <v>0</v>
+        <v>52.900000000000006</v>
       </c>
       <c r="AR3" s="37">
         <f>IFERROR(AS3/$B3,0)</f>
-        <v>0.7259606656580937</v>
+        <v>0.68194402420574873</v>
       </c>
       <c r="AS3" s="33">
         <f>SUM(AS4:AS5)</f>
-        <v>3838.8799999999997</v>
+        <v>3606.1199999999994</v>
       </c>
       <c r="AT3" s="34">
         <f>IFERROR(AU3/$B3,0)</f>
@@ -1794,19 +1794,19 @@
       </c>
       <c r="AV3" s="34">
         <f>IFERROR(AW3/$B3,0)</f>
-        <v>2.4009077155824506E-2</v>
+        <v>2.8010590015128595E-2</v>
       </c>
       <c r="AW3" s="31">
         <f>SUM(AW4:AW5)</f>
-        <v>126.96</v>
+        <v>148.12</v>
       </c>
       <c r="AX3" s="34">
         <f>IFERROR(AY3/$B3,0)</f>
-        <v>4.001512859304085E-3</v>
+        <v>1.0003782148260212E-2</v>
       </c>
       <c r="AY3" s="31">
         <f>SUM(AY4:AY5)</f>
-        <v>21.16</v>
+        <v>52.900000000000006</v>
       </c>
       <c r="AZ3" s="34">
         <f>IFERROR(BA3/$B3,0)</f>
@@ -1818,11 +1818,11 @@
       </c>
       <c r="BB3" s="34">
         <f>IFERROR(BC3/$B3,0)</f>
-        <v>8.8029500756429645E-3</v>
+        <v>2.2808245083207262E-2</v>
       </c>
       <c r="BC3" s="31">
         <f>SUM(BC4:BC5)</f>
-        <v>46.55</v>
+        <v>120.61</v>
       </c>
       <c r="BD3" s="34">
         <f>IFERROR(BE3/$B3,0)</f>
@@ -1935,11 +1935,11 @@
         <v>253.79999999999998</v>
       </c>
       <c r="V4" s="35">
-        <v>5.0000000000000001E-3</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="W4" s="33">
         <f t="shared" ref="W4:W5" si="8">$B4*V4</f>
-        <v>21.150000000000002</v>
+        <v>46.529999999999994</v>
       </c>
       <c r="X4" s="35">
         <v>0</v>
@@ -1984,18 +1984,18 @@
         <v>4.2300000000000004</v>
       </c>
       <c r="AJ4" s="35">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AK4" s="33">
         <f t="shared" ref="AK4:AK5" si="13">$B4*AJ4</f>
-        <v>42.300000000000004</v>
+        <v>21.150000000000002</v>
       </c>
       <c r="AL4" s="35">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="AM4" s="33">
         <f t="shared" ref="AM4:AM5" si="14">$B4*AL4</f>
-        <v>8.4600000000000009</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="AN4" s="35">
         <v>7.0000000000000007E-2</v>
@@ -2117,25 +2117,25 @@
         <v>0</v>
       </c>
       <c r="J5" s="35">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="K5" s="31">
         <f t="shared" si="2"/>
-        <v>10.58</v>
+        <v>31.74</v>
       </c>
       <c r="L5" s="35">
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="M5" s="31">
         <f t="shared" si="3"/>
-        <v>74.06</v>
+        <v>84.64</v>
       </c>
       <c r="N5" s="35">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="O5" s="33">
         <f t="shared" si="4"/>
-        <v>2.1160000000000001</v>
+        <v>1.0580000000000001</v>
       </c>
       <c r="P5" s="35">
         <v>0</v>
@@ -2152,18 +2152,18 @@
         <v>0</v>
       </c>
       <c r="T5" s="39">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="U5" s="33">
         <f t="shared" si="7"/>
-        <v>52.900000000000006</v>
+        <v>63.48</v>
       </c>
       <c r="V5" s="35">
-        <v>5.0000000000000001E-3</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="W5" s="33">
         <f t="shared" si="8"/>
-        <v>5.29</v>
+        <v>26.450000000000003</v>
       </c>
       <c r="X5" s="35">
         <v>0</v>
@@ -2180,67 +2180,67 @@
         <v>0</v>
       </c>
       <c r="AB5" s="35">
-        <v>7.3999999999999996E-2</v>
+        <v>0.13</v>
       </c>
       <c r="AC5" s="31">
         <f t="shared" si="11"/>
-        <v>78.292000000000002</v>
+        <v>137.54</v>
       </c>
       <c r="AD5" s="35">
-        <v>2E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AE5" s="33">
         <f t="shared" si="12"/>
-        <v>2.1160000000000001</v>
+        <v>5.29</v>
       </c>
       <c r="AF5" s="35">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="AG5" s="31">
         <f t="shared" ref="AG5" si="20">$B5*AF5</f>
-        <v>211.60000000000002</v>
+        <v>190.44</v>
       </c>
       <c r="AH5" s="35">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="AI5" s="31">
         <f t="shared" ref="AI5" si="21">$B5*AH5</f>
-        <v>52.900000000000006</v>
+        <v>21.16</v>
       </c>
       <c r="AJ5" s="35">
-        <v>5.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="AK5" s="33">
         <f t="shared" si="13"/>
-        <v>5.29</v>
+        <v>2.1160000000000001</v>
       </c>
       <c r="AL5" s="35">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="AM5" s="33">
         <f t="shared" si="14"/>
-        <v>21.16</v>
+        <v>10.58</v>
       </c>
       <c r="AN5" s="35">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="AO5" s="33">
         <f t="shared" si="15"/>
-        <v>21.16</v>
+        <v>15.87</v>
       </c>
       <c r="AP5" s="35">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="AQ5" s="33">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>52.900000000000006</v>
       </c>
       <c r="AR5" s="35">
-        <v>0.31</v>
+        <v>0.09</v>
       </c>
       <c r="AS5" s="33">
         <f t="shared" si="17"/>
-        <v>327.98</v>
+        <v>95.22</v>
       </c>
       <c r="AT5" s="35">
         <v>0</v>
@@ -2250,18 +2250,18 @@
         <v>0</v>
       </c>
       <c r="AV5" s="35">
-        <v>0.12</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="AW5" s="31">
         <f t="shared" ref="AW5" si="23">$B5*AV5</f>
-        <v>126.96</v>
+        <v>148.12</v>
       </c>
       <c r="AX5" s="35">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="AY5" s="31">
         <f t="shared" ref="AY5" si="24">$B5*AX5</f>
-        <v>21.16</v>
+        <v>52.900000000000006</v>
       </c>
       <c r="AZ5" s="35">
         <v>0</v>
@@ -2271,11 +2271,11 @@
         <v>0</v>
       </c>
       <c r="BB5" s="35">
-        <v>0.04</v>
+        <v>0.11</v>
       </c>
       <c r="BC5" s="31">
         <f t="shared" si="25"/>
-        <v>42.32</v>
+        <v>116.38</v>
       </c>
       <c r="BD5" s="35">
         <v>0</v>
@@ -12657,11 +12657,11 @@
         <f>IFERROR(SUM(F51,H51,J51,L51,N51,P51,R51,T51,V51,X51,Z51,AB51,AD51,AF51,AH51,AJ51,AL51,AN51,AP51,AR51,AT51,AV51,AX51,AZ51,BB51,BD51,BF51,BH51,BJ51,BL51),0)</f>
         <v>1</v>
       </c>
-      <c r="D51" s="53">
+      <c r="D51" s="55">
         <f>SUM(D52,D56,D62,D68,D86,D100,D111)</f>
         <v>0</v>
       </c>
-      <c r="E51" s="54"/>
+      <c r="E51" s="56"/>
       <c r="F51" s="34">
         <f>IFERROR(G51/$B51,0)</f>
         <v>2.526813531299273E-3</v>
@@ -29735,24 +29735,6 @@
     <sortCondition ref="A32"/>
   </sortState>
   <mergeCells count="34">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="BB1:BC1"/>
-    <mergeCell ref="BD1:BE1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D51:E51"/>
     <mergeCell ref="BH1:BI1"/>
     <mergeCell ref="BJ1:BK1"/>
     <mergeCell ref="BL1:BM1"/>
@@ -29769,6 +29751,24 @@
     <mergeCell ref="AJ1:AK1"/>
     <mergeCell ref="AD1:AE1"/>
     <mergeCell ref="AZ1:BA1"/>
+    <mergeCell ref="BB1:BC1"/>
+    <mergeCell ref="BD1:BE1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates to MP and religion.
</commit_message>
<xml_diff>
--- a/development/tools/PopulationCalculator.xlsx
+++ b/development/tools/PopulationCalculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/Documents/GitHub/Atlas-Exandria/development/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC37D24-109D-634A-B521-C4BB08BB8017}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C780BE33-9B18-6841-928C-FBEF84B52143}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="1100" windowWidth="49540" windowHeight="27700" tabRatio="918" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="918" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population" sheetId="14" r:id="rId1"/>
@@ -810,7 +810,16 @@
     <xf numFmtId="10" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="9" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -819,13 +828,10 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -834,20 +840,14 @@
     <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="9" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="9" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1133,9 +1133,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BM126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomLeft" activeCell="AR62" sqref="AR62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -1211,136 +1211,136 @@
       <c r="A1" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="51">
+      <c r="B1" s="43">
         <f>SUM(B51,B2)</f>
         <v>2524854</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="47">
+      <c r="C1" s="44"/>
+      <c r="D1" s="50">
         <f>SUM(D2,D51)</f>
         <v>2042171.4</v>
       </c>
-      <c r="E1" s="48"/>
-      <c r="F1" s="43" t="s">
+      <c r="E1" s="44"/>
+      <c r="F1" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43" t="s">
+      <c r="G1" s="49"/>
+      <c r="H1" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43" t="s">
+      <c r="I1" s="49"/>
+      <c r="J1" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43" t="s">
+      <c r="K1" s="49"/>
+      <c r="L1" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="43"/>
-      <c r="N1" s="44" t="s">
+      <c r="M1" s="49"/>
+      <c r="N1" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="45"/>
-      <c r="P1" s="44" t="s">
+      <c r="O1" s="48"/>
+      <c r="P1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="52" t="s">
+      <c r="Q1" s="48"/>
+      <c r="R1" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="S1" s="53"/>
-      <c r="T1" s="44" t="s">
+      <c r="S1" s="46"/>
+      <c r="T1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="U1" s="45"/>
-      <c r="V1" s="44" t="s">
+      <c r="U1" s="48"/>
+      <c r="V1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="45"/>
-      <c r="X1" s="43" t="s">
+      <c r="W1" s="48"/>
+      <c r="X1" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" s="43"/>
-      <c r="Z1" s="43" t="s">
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" s="43"/>
-      <c r="AB1" s="43" t="s">
+      <c r="AA1" s="49"/>
+      <c r="AB1" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="AC1" s="43"/>
-      <c r="AD1" s="44" t="s">
+      <c r="AC1" s="49"/>
+      <c r="AD1" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="AE1" s="45"/>
-      <c r="AF1" s="43" t="s">
+      <c r="AE1" s="48"/>
+      <c r="AF1" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="43"/>
-      <c r="AH1" s="52" t="s">
+      <c r="AG1" s="49"/>
+      <c r="AH1" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="44" t="s">
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="AK1" s="45"/>
-      <c r="AL1" s="44" t="s">
+      <c r="AK1" s="48"/>
+      <c r="AL1" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="AM1" s="45"/>
-      <c r="AN1" s="44" t="s">
+      <c r="AM1" s="48"/>
+      <c r="AN1" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="AO1" s="45"/>
-      <c r="AP1" s="46" t="s">
+      <c r="AO1" s="48"/>
+      <c r="AP1" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="AQ1" s="46"/>
-      <c r="AR1" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="AS1" s="45"/>
-      <c r="AT1" s="43" t="s">
+      <c r="AQ1" s="55"/>
+      <c r="AR1" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS1" s="48"/>
+      <c r="AT1" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="AU1" s="43"/>
-      <c r="AV1" s="43" t="s">
+      <c r="AU1" s="49"/>
+      <c r="AV1" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="AW1" s="43"/>
-      <c r="AX1" s="43" t="s">
+      <c r="AW1" s="49"/>
+      <c r="AX1" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="AY1" s="43"/>
-      <c r="AZ1" s="43" t="s">
+      <c r="AY1" s="49"/>
+      <c r="AZ1" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="BA1" s="43"/>
-      <c r="BB1" s="43" t="s">
+      <c r="BA1" s="49"/>
+      <c r="BB1" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="BC1" s="43"/>
-      <c r="BD1" s="43" t="s">
+      <c r="BC1" s="49"/>
+      <c r="BD1" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="BE1" s="43"/>
-      <c r="BF1" s="44" t="s">
+      <c r="BE1" s="49"/>
+      <c r="BF1" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="BG1" s="45"/>
-      <c r="BH1" s="43" t="s">
+      <c r="BG1" s="48"/>
+      <c r="BH1" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="BI1" s="43"/>
-      <c r="BJ1" s="43" t="s">
+      <c r="BI1" s="49"/>
+      <c r="BJ1" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="BK1" s="43"/>
-      <c r="BL1" s="43" t="s">
+      <c r="BK1" s="49"/>
+      <c r="BL1" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="BM1" s="43"/>
+      <c r="BM1" s="49"/>
     </row>
     <row r="2" spans="1:65" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -1354,53 +1354,53 @@
         <f>IFERROR(SUM(F2,H2,J2,L2,N2,P2,R2,T2,V2,X2,Z2,AB2,AD2,AF2,AH2,AJ2,AL2,AN2,AP2,AR2,AT2,AV2,AX2,AZ2,BB2,BD2,BF2,BH2,BJ2,BL2),0)</f>
         <v>1.0000000000000002</v>
       </c>
-      <c r="D2" s="49">
+      <c r="D2" s="51">
         <f>SUM(E46,E42,E33,E27,E22,E13,E6,E3)</f>
         <v>969573.6</v>
       </c>
-      <c r="E2" s="50">
+      <c r="E2" s="52">
         <f>SUM(E46,E42,E33,E27,E22,E13,E6,E3)</f>
         <v>969573.6</v>
       </c>
       <c r="F2" s="32">
         <f>IFERROR(G2/$B2,0)</f>
-        <v>2.4481440488134161E-4</v>
+        <v>2.8735811842489596E-4</v>
       </c>
       <c r="G2" s="29">
         <f>SUM(G46,G42,G33,G27,G22,G13,G6,G3)</f>
-        <v>250.60499999999999</v>
+        <v>294.15500000000003</v>
       </c>
       <c r="H2" s="32">
         <f>IFERROR(I2/$B2,0)</f>
-        <v>2.9802848230796961E-3</v>
+        <v>3.0954825512160859E-3</v>
       </c>
       <c r="I2" s="29">
         <f>SUM(I46,I42,I33,I27,I22,I13,I6,I3)</f>
-        <v>3050.7775000000001</v>
+        <v>3168.7</v>
       </c>
       <c r="J2" s="32">
         <f>IFERROR(K2/$B2,0)</f>
-        <v>1.2529885615535731E-2</v>
+        <v>1.3380759886406817E-2</v>
       </c>
       <c r="K2" s="29">
         <f>SUM(K46,K42,K33,K27,K22,K13,K6,K3)</f>
-        <v>12826.254999999997</v>
+        <v>13697.254999999997</v>
       </c>
       <c r="L2" s="32">
         <f>IFERROR(M2/$B2,0)</f>
-        <v>1.413410110652731E-3</v>
+        <v>1.6054063242133807E-3</v>
       </c>
       <c r="M2" s="29">
         <f>SUM(M46,M42,M33,M27,M22,M13,M6,M3)</f>
-        <v>1446.8415</v>
+        <v>1643.3789999999999</v>
       </c>
       <c r="N2" s="35">
         <f>IFERROR(O2/$B2,0)</f>
-        <v>3.6471382392275508E-3</v>
+        <v>3.6556469819362617E-3</v>
       </c>
       <c r="O2" s="31">
         <f>SUM(O46,O42,O33,O27,O22,O13,O6,O3)</f>
-        <v>3733.404</v>
+        <v>3742.114</v>
       </c>
       <c r="P2" s="35">
         <f>IFERROR(Q2/$B2,0)</f>
@@ -1412,27 +1412,27 @@
       </c>
       <c r="R2" s="32">
         <f>IFERROR(S2/$B2,0)</f>
-        <v>8.1096697806776318E-3</v>
+        <v>8.5351069161131738E-3</v>
       </c>
       <c r="S2" s="29">
         <f>SUM(S46,S42,S33,S27,S22,S13,S6,S3)</f>
-        <v>8301.487799999999</v>
+        <v>8736.987799999999</v>
       </c>
       <c r="T2" s="36">
         <f>IFERROR(U2/$B2,0)</f>
-        <v>9.997108199751284E-2</v>
+        <v>9.8186444039142187E-2</v>
       </c>
       <c r="U2" s="31">
         <f>SUM(U46,U42,U33,U27,U22,U13,U6,U3)</f>
-        <v>102335.698</v>
+        <v>100508.84800000001</v>
       </c>
       <c r="V2" s="35">
         <f>IFERROR(W2/$B2,0)</f>
-        <v>9.7557571755272549E-2</v>
+        <v>9.0562818650460647E-2</v>
       </c>
       <c r="W2" s="31">
         <f>SUM(W46,W42,W33,W27,W22,W13,W6,W3)</f>
-        <v>99865.10100000001</v>
+        <v>92704.900999999998</v>
       </c>
       <c r="X2" s="32">
         <f>IFERROR(Y2/$B2,0)</f>
@@ -1444,67 +1444,67 @@
       </c>
       <c r="Z2" s="32">
         <f>IFERROR(AA2/$B2,0)</f>
-        <v>9.7460272182077327E-4</v>
+        <v>1.1281996926692931E-3</v>
       </c>
       <c r="AA2" s="29">
         <f>SUM(AA46,AA42,AA33,AA27,AA22,AA13,AA6,AA3)</f>
-        <v>997.65499999999997</v>
+        <v>1154.885</v>
       </c>
       <c r="AB2" s="32">
         <f>IFERROR(AC2/$B2,0)</f>
-        <v>3.4610580929279743E-3</v>
+        <v>5.5467990617914477E-3</v>
       </c>
       <c r="AC2" s="29">
         <f>SUM(AC46,AC42,AC33,AC27,AC22,AC13,AC6,AC3)</f>
-        <v>3542.9224999999997</v>
+        <v>5677.9975000000004</v>
       </c>
       <c r="AD2" s="35">
         <f>IFERROR(AE2/$B2,0)</f>
-        <v>3.699998046212926E-2</v>
+        <v>3.4707015951694571E-2</v>
       </c>
       <c r="AE2" s="31">
         <f>SUM(AE46,AE42,AE33,AE27,AE22,AE13,AE6,AE3)</f>
-        <v>37875.141000000003</v>
+        <v>35527.941000000006</v>
       </c>
       <c r="AF2" s="32">
         <f>IFERROR(AG2/$B2,0)</f>
-        <v>3.411127598903145E-2</v>
+        <v>3.5736226045349352E-2</v>
       </c>
       <c r="AG2" s="29">
         <f>SUM(AG46,AG42,AG33,AG27,AG22,AG13,AG6,AG3)</f>
-        <v>34918.110000000008</v>
+        <v>36581.495000000003</v>
       </c>
       <c r="AH2" s="32">
         <f>IFERROR(AI2/$B2,0)</f>
-        <v>2.7555475341741781E-3</v>
+        <v>2.6787490487499184E-3</v>
       </c>
       <c r="AI2" s="29">
         <f>SUM(AI46,AI42,AI33,AI27,AI22,AI13,AI6,AI3)</f>
-        <v>2820.7244999999998</v>
+        <v>2742.1095</v>
       </c>
       <c r="AJ2" s="35">
         <f>IFERROR(AK2/$B2,0)</f>
-        <v>4.8082737021236686E-2</v>
+        <v>4.6505322604437252E-2</v>
       </c>
       <c r="AK2" s="31">
         <f>SUM(AK46,AK42,AK33,AK27,AK22,AK13,AK6,AK3)</f>
-        <v>49220.038</v>
+        <v>47605.313000000009</v>
       </c>
       <c r="AL2" s="35">
         <f>IFERROR(AM2/$B2,0)</f>
-        <v>3.0334017972887296E-2</v>
+        <v>2.9483143702016209E-2</v>
       </c>
       <c r="AM2" s="31">
         <f>SUM(AM46,AM42,AM33,AM27,AM22,AM13,AM6,AM3)</f>
-        <v>31051.5085</v>
+        <v>30180.5085</v>
       </c>
       <c r="AN2" s="35">
         <f>IFERROR(AO2/$B2,0)</f>
-        <v>5.2801374098449379E-2</v>
+        <v>5.1525062692142749E-2</v>
       </c>
       <c r="AO2" s="31">
         <f>SUM(AO46,AO42,AO33,AO27,AO22,AO13,AO6,AO3)</f>
-        <v>54050.285000000003</v>
+        <v>52743.785000000003</v>
       </c>
       <c r="AP2" s="35">
         <f>IFERROR(AQ2/$B2,0)</f>
@@ -1516,67 +1516,67 @@
       </c>
       <c r="AR2" s="35">
         <f>IFERROR(AS2/$B2,0)</f>
-        <v>0.36582509405042529</v>
+        <v>0.36642730007141094</v>
       </c>
       <c r="AS2" s="31">
         <f>SUM(AS46,AS42,AS33,AS27,AS22,AS13,AS6,AS3)</f>
-        <v>374477.95500000002</v>
+        <v>375094.40500000003</v>
       </c>
       <c r="AT2" s="32">
         <f>IFERROR(AU2/$B2,0)</f>
-        <v>2.8090573661191833E-5</v>
+        <v>1.1317800074830046E-4</v>
       </c>
       <c r="AU2" s="29">
         <f>SUM(AU46,AU42,AU33,AU27,AU22,AU13,AU6,AU3)</f>
-        <v>28.755000000000003</v>
+        <v>115.85500000000002</v>
       </c>
       <c r="AV2" s="32">
         <f>IFERROR(AW2/$B2,0)</f>
-        <v>6.2676854363734585E-3</v>
+        <v>9.2810991615322781E-3</v>
       </c>
       <c r="AW2" s="29">
         <f>SUM(AW46,AW42,AW33,AW27,AW22,AW13,AW6,AW3)</f>
-        <v>6415.9349999999995</v>
+        <v>9500.6250000000018</v>
       </c>
       <c r="AX2" s="32">
         <f>IFERROR(AY2/$B2,0)</f>
-        <v>7.3520563120510569E-3</v>
+        <v>9.225078713196758E-3</v>
       </c>
       <c r="AY2" s="29">
         <f>SUM(AY46,AY42,AY33,AY27,AY22,AY13,AY6,AY3)</f>
-        <v>7525.9545000000007</v>
+        <v>9443.2795000000006</v>
       </c>
       <c r="AZ2" s="32">
         <f>IFERROR(BA2/$B2,0)</f>
-        <v>4.3448805405738077E-4</v>
+        <v>5.1106673843577847E-4</v>
       </c>
       <c r="BA2" s="29">
         <f>SUM(BA46,BA42,BA33,BA27,BA22,BA13,BA6,BA3)</f>
-        <v>444.76499999999999</v>
+        <v>523.15499999999997</v>
       </c>
       <c r="BB2" s="32">
         <f>IFERROR(BC2/$B2,0)</f>
-        <v>1.4444336117805547E-2</v>
+        <v>1.8532928638904003E-2</v>
       </c>
       <c r="BC2" s="29">
         <f>SUM(BC46,BC42,BC33,BC27,BC22,BC13,BC6,BC3)</f>
-        <v>14785.988000000001</v>
+        <v>18971.288</v>
       </c>
       <c r="BD2" s="32">
         <f>IFERROR(BE2/$B2,0)</f>
-        <v>1.2114213019450929E-2</v>
+        <v>1.2498205446572225E-2</v>
       </c>
       <c r="BE2" s="29">
         <f>SUM(BE46,BE42,BE33,BE27,BE22,BE13,BE6,BE3)</f>
-        <v>12400.750500000002</v>
+        <v>12793.825499999999</v>
       </c>
       <c r="BF2" s="35">
         <f>IFERROR(BG2/$B2,0)</f>
-        <v>3.4124776657715065E-2</v>
+        <v>3.3356791803472466E-2</v>
       </c>
       <c r="BG2" s="31">
         <f>SUM(BG46,BG42,BG33,BG27,BG22,BG13,BG6,BG3)</f>
-        <v>34931.93</v>
+        <v>34145.78</v>
       </c>
       <c r="BH2" s="32">
         <f>IFERROR(BI2/$B2,0)</f>
@@ -3915,7 +3915,7 @@
         <v>215.66249999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:65" ht="16" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:65" ht="14" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>46</v>
       </c>
@@ -3925,7 +3925,7 @@
       </c>
       <c r="C13" s="40">
         <f>IFERROR(SUM(F13,H13,J13,L13,N13,P13,R13,T13,V13,X13,Z13,AB13,AD13,AF13,AH13,AJ13,AL13,AN13,AP13,AR13,AT13,AV13,AX13,AZ13,BB13,BD13,BF13,BH13,BJ13,BL13),0)</f>
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D13" s="26">
         <v>328</v>
@@ -3936,11 +3936,11 @@
       </c>
       <c r="F13" s="32">
         <f>IFERROR(G13/$B13,0)</f>
-        <v>1.4291902677229437E-3</v>
+        <v>1.7150283212675327E-3</v>
       </c>
       <c r="G13" s="29">
         <f>SUM(G14:G21)</f>
-        <v>217.75</v>
+        <v>261.3</v>
       </c>
       <c r="H13" s="32">
         <f>IFERROR(I13/$B13,0)</f>
@@ -3952,11 +3952,11 @@
       </c>
       <c r="J13" s="32">
         <f>IFERROR(K13/$B13,0)</f>
-        <v>5.716761070891775E-3</v>
+        <v>1.143352214178355E-2</v>
       </c>
       <c r="K13" s="29">
         <f>SUM(K14:K21)</f>
-        <v>871</v>
+        <v>1742</v>
       </c>
       <c r="L13" s="32">
         <f>IFERROR(M13/$B13,0)</f>
@@ -3968,11 +3968,11 @@
       </c>
       <c r="N13" s="35">
         <f>IFERROR(O13/$B13,0)</f>
-        <v>5.8875813046817055E-3</v>
+        <v>5.9447489153906232E-3</v>
       </c>
       <c r="O13" s="31">
         <f>SUM(O14:O21)</f>
-        <v>897.02599999999995</v>
+        <v>905.73599999999999</v>
       </c>
       <c r="P13" s="35">
         <f>IFERROR(Q13/$B13,0)</f>
@@ -3984,27 +3984,27 @@
       </c>
       <c r="R13" s="32">
         <f>IFERROR(S13/$B13,0)</f>
-        <v>5.1818501040306116E-2</v>
+        <v>5.4676881575752005E-2</v>
       </c>
       <c r="S13" s="29">
         <f>SUM(S14:S21)</f>
-        <v>7895.0149999999994</v>
+        <v>8330.5149999999994</v>
       </c>
       <c r="T13" s="36">
         <f>IFERROR(U13/$B13,0)</f>
-        <v>0.42504453297803219</v>
+        <v>0.40789424976535693</v>
       </c>
       <c r="U13" s="31">
         <f>SUM(U14:U21)</f>
-        <v>64759.360000000008</v>
+        <v>62146.360000000015</v>
       </c>
       <c r="V13" s="35">
         <f>IFERROR(W13/$B13,0)</f>
-        <v>4.8588701684836477E-2</v>
+        <v>4.2871940613944698E-2</v>
       </c>
       <c r="W13" s="31">
         <f>SUM(W14:W21)</f>
-        <v>7402.9260000000004</v>
+        <v>6531.9260000000004</v>
       </c>
       <c r="X13" s="32">
         <f>IFERROR(Y13/$B13,0)</f>
@@ -4024,27 +4024,27 @@
       </c>
       <c r="AB13" s="32">
         <f>IFERROR(AC13/$B13,0)</f>
-        <v>2.8583805354458875E-3</v>
+        <v>1.4291902677229438E-2</v>
       </c>
       <c r="AC13" s="29">
         <f>SUM(AC14:AC21)</f>
-        <v>435.5</v>
+        <v>2177.5</v>
       </c>
       <c r="AD13" s="35">
         <f>IFERROR(AE13/$B13,0)</f>
-        <v>8.7341771736490784E-2</v>
+        <v>6.1616346917477804E-2</v>
       </c>
       <c r="AE13" s="31">
         <f>SUM(AE14:AE21)</f>
-        <v>13307.305</v>
+        <v>9387.8050000000003</v>
       </c>
       <c r="AF13" s="32">
         <f>IFERROR(AG13/$B13,0)</f>
-        <v>8.0608480627990475E-2</v>
+        <v>9.204200276977402E-2</v>
       </c>
       <c r="AG13" s="29">
         <f>SUM(AG14:AG21)</f>
-        <v>12281.427500000002</v>
+        <v>14023.4275</v>
       </c>
       <c r="AH13" s="32">
         <f>IFERROR(AI13/$B13,0)</f>
@@ -4056,27 +4056,27 @@
       </c>
       <c r="AJ13" s="35">
         <f>IFERROR(AK13/$B13,0)</f>
-        <v>2.2730557433430252E-2</v>
+        <v>1.9872176897984366E-2</v>
       </c>
       <c r="AK13" s="31">
         <f>SUM(AK14:AK21)</f>
-        <v>3463.2049999999999</v>
+        <v>3027.7049999999999</v>
       </c>
       <c r="AL13" s="35">
         <f>IFERROR(AM13/$B13,0)</f>
-        <v>3.6466286861951046E-2</v>
+        <v>3.0749525791059273E-2</v>
       </c>
       <c r="AM13" s="31">
         <f>SUM(AM14:AM21)</f>
-        <v>5555.9669999999996</v>
+        <v>4684.9669999999996</v>
       </c>
       <c r="AN13" s="35">
         <f>IFERROR(AO13/$B13,0)</f>
-        <v>2.9061492921323977E-2</v>
+        <v>2.0486351314986318E-2</v>
       </c>
       <c r="AO13" s="31">
         <f>SUM(AO14:AO21)</f>
-        <v>4427.78</v>
+        <v>3121.28</v>
       </c>
       <c r="AP13" s="35">
         <f>IFERROR(AQ13/$B13,0)</f>
@@ -4088,51 +4088,51 @@
       </c>
       <c r="AR13" s="35">
         <f>IFERROR(AS13/$B13,0)</f>
-        <v>9.737580320164875E-2</v>
+        <v>8.5942281059865192E-2</v>
       </c>
       <c r="AS13" s="31">
         <f>SUM(AS14:AS21)</f>
-        <v>14836.080000000002</v>
+        <v>13094.080000000002</v>
       </c>
       <c r="AT13" s="32">
         <f>IFERROR(AU13/$B13,0)</f>
-        <v>0</v>
+        <v>5.7167610708917761E-4</v>
       </c>
       <c r="AU13" s="29">
         <f>SUM(AU14:AU21)</f>
-        <v>0</v>
+        <v>87.100000000000009</v>
       </c>
       <c r="AV13" s="32">
         <f>IFERROR(AW13/$B13,0)</f>
-        <v>2.338155277994736E-2</v>
+        <v>4.0531835992622695E-2</v>
       </c>
       <c r="AW13" s="29">
         <f>SUM(AW14:AW21)</f>
-        <v>3562.39</v>
+        <v>6175.3900000000012</v>
       </c>
       <c r="AX13" s="32">
         <f>IFERROR(AY13/$B13,0)</f>
-        <v>1.4291902677229437E-3</v>
+        <v>1.143352214178355E-2</v>
       </c>
       <c r="AY13" s="29">
         <f>SUM(AY14:AY21)</f>
-        <v>217.75</v>
+        <v>1742</v>
       </c>
       <c r="AZ13" s="32">
         <f>IFERROR(BA13/$B13,0)</f>
-        <v>5.7167610708917759E-5</v>
+        <v>5.7167610708917761E-4</v>
       </c>
       <c r="BA13" s="29">
         <f>SUM(BA14:BA21)</f>
-        <v>8.7100000000000009</v>
+        <v>87.100000000000009</v>
       </c>
       <c r="BB13" s="32">
         <f>IFERROR(BC13/$B13,0)</f>
-        <v>3.463521025997808E-2</v>
+        <v>5.1785493472653404E-2</v>
       </c>
       <c r="BC13" s="29">
         <f>SUM(BC14:BC21)</f>
-        <v>5276.9859999999999</v>
+        <v>7889.9859999999999</v>
       </c>
       <c r="BD13" s="32">
         <f>IFERROR(BE13/$B13,0)</f>
@@ -5752,16 +5752,16 @@
       </c>
       <c r="C21" s="40">
         <f t="shared" si="82"/>
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="16"/>
       <c r="F21" s="33">
-        <v>2.5000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="G21" s="29">
         <f t="shared" si="63"/>
-        <v>217.75</v>
+        <v>261.3</v>
       </c>
       <c r="H21" s="33">
         <v>5.0000000000000001E-3</v>
@@ -5771,11 +5771,11 @@
         <v>435.5</v>
       </c>
       <c r="J21" s="33">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="K21" s="29">
         <f t="shared" si="65"/>
-        <v>871</v>
+        <v>1742</v>
       </c>
       <c r="L21" s="33">
         <v>0</v>
@@ -5785,11 +5785,11 @@
         <v>0</v>
       </c>
       <c r="N21" s="33">
-        <v>4.8999999999999998E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="O21" s="31">
         <f t="shared" si="67"/>
-        <v>426.78999999999996</v>
+        <v>435.5</v>
       </c>
       <c r="P21" s="33">
         <v>1.4999999999999999E-2</v>
@@ -5799,25 +5799,25 @@
         <v>1306.5</v>
       </c>
       <c r="R21" s="33">
-        <v>5.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="S21" s="29">
         <f t="shared" si="69"/>
-        <v>435.5</v>
+        <v>871</v>
       </c>
       <c r="T21" s="37">
-        <v>0.31</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="U21" s="31">
         <f t="shared" si="70"/>
-        <v>27001</v>
+        <v>24388.000000000004</v>
       </c>
       <c r="V21" s="33">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="W21" s="31">
         <f t="shared" si="71"/>
-        <v>1742</v>
+        <v>871</v>
       </c>
       <c r="X21" s="33">
         <v>5.0000000000000001E-3</v>
@@ -5834,25 +5834,25 @@
         <v>435.5</v>
       </c>
       <c r="AB21" s="33">
-        <v>5.0000000000000001E-3</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AC21" s="29">
         <f t="shared" si="74"/>
-        <v>435.5</v>
+        <v>2177.5</v>
       </c>
       <c r="AD21" s="33">
-        <v>0.1</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AE21" s="31">
         <f t="shared" si="75"/>
-        <v>8710</v>
+        <v>4790.5</v>
       </c>
       <c r="AF21" s="33">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="AG21" s="29">
         <f t="shared" si="83"/>
-        <v>12194.000000000002</v>
+        <v>13936</v>
       </c>
       <c r="AH21" s="33">
         <v>0.01</v>
@@ -5862,25 +5862,25 @@
         <v>871</v>
       </c>
       <c r="AJ21" s="33">
-        <v>0.03</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AK21" s="31">
         <f t="shared" si="76"/>
-        <v>2613</v>
+        <v>2177.5</v>
       </c>
       <c r="AL21" s="33">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="AM21" s="31">
         <f t="shared" si="77"/>
-        <v>5226</v>
+        <v>4355</v>
       </c>
       <c r="AN21" s="33">
-        <v>0.04</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AO21" s="31">
         <f t="shared" si="78"/>
-        <v>3484</v>
+        <v>2177.5</v>
       </c>
       <c r="AP21" s="33">
         <v>0.02</v>
@@ -5890,46 +5890,46 @@
         <v>1742</v>
       </c>
       <c r="AR21" s="33">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="AS21" s="31">
         <f t="shared" si="80"/>
-        <v>8710</v>
+        <v>6968</v>
       </c>
       <c r="AT21" s="33">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="AU21" s="29">
         <f t="shared" si="85"/>
-        <v>0</v>
+        <v>87.100000000000009</v>
       </c>
       <c r="AV21" s="33">
-        <v>0.04</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="AW21" s="29">
         <f t="shared" si="86"/>
-        <v>3484</v>
+        <v>6097.0000000000009</v>
       </c>
       <c r="AX21" s="33">
-        <v>2.5000000000000001E-3</v>
+        <v>0.02</v>
       </c>
       <c r="AY21" s="29">
         <f t="shared" si="87"/>
-        <v>217.75</v>
+        <v>1742</v>
       </c>
       <c r="AZ21" s="33">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="BA21" s="29">
         <f t="shared" si="88"/>
-        <v>8.7100000000000009</v>
+        <v>87.100000000000009</v>
       </c>
       <c r="BB21" s="33">
-        <v>0.06</v>
+        <v>0.09</v>
       </c>
       <c r="BC21" s="29">
         <f t="shared" si="88"/>
-        <v>5226</v>
+        <v>7839</v>
       </c>
       <c r="BD21" s="33">
         <v>0</v>
@@ -5996,11 +5996,11 @@
       </c>
       <c r="H22" s="32">
         <f>IFERROR(I22/$B22,0)</f>
-        <v>1E-3</v>
+        <v>2.0325872803215383E-3</v>
       </c>
       <c r="I22" s="29">
         <f>SUM(I23:I26)</f>
-        <v>114.20099999999999</v>
+        <v>232.12349999999998</v>
       </c>
       <c r="J22" s="32">
         <f>IFERROR(K22/$B22,0)</f>
@@ -6012,11 +6012,11 @@
       </c>
       <c r="L22" s="32">
         <f>IFERROR(M22/$B22,0)</f>
-        <v>3.6388341608217089E-3</v>
+        <v>5.3598129613576066E-3</v>
       </c>
       <c r="M22" s="29">
         <f>SUM(M23:M26)</f>
-        <v>415.55849999999998</v>
+        <v>612.096</v>
       </c>
       <c r="N22" s="35">
         <f>IFERROR(O22/$B22,0)</f>
@@ -6044,19 +6044,19 @@
       </c>
       <c r="T22" s="36">
         <f>IFERROR(U22/$B22,0)</f>
-        <v>7.428954212309874E-2</v>
+        <v>8.1173457325242337E-2</v>
       </c>
       <c r="U22" s="31">
         <f>SUM(U23:U26)</f>
-        <v>8483.9399999999987</v>
+        <v>9270.09</v>
       </c>
       <c r="V22" s="35">
         <f>IFERROR(W22/$B22,0)</f>
-        <v>9.0932960306827418E-2</v>
+        <v>3.5861638689678725E-2</v>
       </c>
       <c r="W22" s="31">
         <f>SUM(W23:W26)</f>
-        <v>10384.634999999998</v>
+        <v>4095.4349999999999</v>
       </c>
       <c r="X22" s="32">
         <f>IFERROR(Y22/$B22,0)</f>
@@ -6068,51 +6068,51 @@
       </c>
       <c r="Z22" s="32">
         <f>IFERROR(AA22/$B22,0)</f>
-        <v>9.4420364094885325E-4</v>
+        <v>2.3209866813775708E-3</v>
       </c>
       <c r="AA22" s="29">
         <f>SUM(AA23:AA26)</f>
-        <v>107.82899999999999</v>
+        <v>265.05899999999997</v>
       </c>
       <c r="AB22" s="32">
         <f>IFERROR(AC22/$B22,0)</f>
-        <v>1.8238062713986741E-2</v>
+        <v>2.168002031505854E-2</v>
       </c>
       <c r="AC22" s="29">
         <f>SUM(AC23:AC26)</f>
-        <v>2082.8049999999998</v>
+        <v>2475.88</v>
       </c>
       <c r="AD22" s="35">
         <f>IFERROR(AE22/$B22,0)</f>
-        <v>3.819887741788601E-2</v>
+        <v>5.1966707822173185E-2</v>
       </c>
       <c r="AE22" s="31">
         <f>SUM(AE23:AE26)</f>
-        <v>4362.3500000000004</v>
+        <v>5934.65</v>
       </c>
       <c r="AF22" s="32">
         <f>IFERROR(AG22/$B22,0)</f>
-        <v>1.1140335898985122E-2</v>
+        <v>1.0451944378770766E-2</v>
       </c>
       <c r="AG22" s="29">
         <f>SUM(AG23:AG26)</f>
-        <v>1272.2375</v>
+        <v>1193.6225000000002</v>
       </c>
       <c r="AH22" s="32">
         <f>IFERROR(AI22/$B22,0)</f>
-        <v>8.271582560573025E-3</v>
+        <v>7.5831910403586665E-3</v>
       </c>
       <c r="AI22" s="29">
         <f>SUM(AI23:AI26)</f>
-        <v>944.62300000000005</v>
+        <v>866.00800000000004</v>
       </c>
       <c r="AJ22" s="35">
         <f>IFERROR(AK22/$B22,0)</f>
-        <v>3.2148930394655037E-2</v>
+        <v>2.1823057591439658E-2</v>
       </c>
       <c r="AK22" s="31">
         <f>SUM(AK23:AK26)</f>
-        <v>3671.44</v>
+        <v>2492.2150000000001</v>
       </c>
       <c r="AL22" s="35">
         <f>IFERROR(AM22/$B22,0)</f>
@@ -6140,11 +6140,11 @@
       </c>
       <c r="AR22" s="35">
         <f>IFERROR(AS22/$B22,0)</f>
-        <v>0.46668925841279851</v>
+        <v>0.48734100401922925</v>
       </c>
       <c r="AS22" s="31">
         <f>SUM(AS23:AS26)</f>
-        <v>53296.380000000005</v>
+        <v>55654.83</v>
       </c>
       <c r="AT22" s="32">
         <f>IFERROR(AU22/$B22,0)</f>
@@ -6156,19 +6156,19 @@
       </c>
       <c r="AV22" s="32">
         <f>IFERROR(AW22/$B22,0)</f>
-        <v>1.3767830404287178E-3</v>
+        <v>5.5071321617148712E-3</v>
       </c>
       <c r="AW22" s="29">
         <f>SUM(AW23:AW26)</f>
-        <v>157.22999999999999</v>
+        <v>628.91999999999996</v>
       </c>
       <c r="AX22" s="32">
         <f>IFERROR(AY22/$B22,0)</f>
-        <v>1.5645440933091653E-3</v>
+        <v>5.0065016943809607E-3</v>
       </c>
       <c r="AY22" s="29">
         <f>SUM(AY23:AY26)</f>
-        <v>178.67249999999999</v>
+        <v>571.74750000000006</v>
       </c>
       <c r="AZ22" s="32">
         <f>IFERROR(BA22/$B22,0)</f>
@@ -6180,27 +6180,27 @@
       </c>
       <c r="BB22" s="32">
         <f>IFERROR(BC22/$B22,0)</f>
-        <v>1.5555336643286836E-2</v>
+        <v>2.9323167047574011E-2</v>
       </c>
       <c r="BC22" s="29">
         <f>SUM(BC23:BC26)</f>
-        <v>1776.4349999999999</v>
+        <v>3348.7349999999997</v>
       </c>
       <c r="BD22" s="32">
         <f>IFERROR(BE22/$B22,0)</f>
-        <v>3.8211399199656743E-3</v>
+        <v>7.2630975210374689E-3</v>
       </c>
       <c r="BE22" s="29">
         <f>SUM(BE23:BE26)</f>
-        <v>436.37799999999999</v>
+        <v>829.45299999999997</v>
       </c>
       <c r="BF22" s="35">
         <f>IFERROR(BG22/$B22,0)</f>
-        <v>4.4647726377177087E-2</v>
+        <v>3.7763811175033496E-2</v>
       </c>
       <c r="BG22" s="31">
         <f>SUM(BG23:BG26)</f>
-        <v>5098.8150000000005</v>
+        <v>4312.665</v>
       </c>
       <c r="BH22" s="32">
         <f>IFERROR(BI22/$B22,0)</f>
@@ -6908,7 +6908,7 @@
       </c>
       <c r="C26" s="40">
         <f t="shared" si="118"/>
-        <v>1.0000000000000002</v>
+        <v>1</v>
       </c>
       <c r="D26" s="17"/>
       <c r="E26" s="18"/>
@@ -6920,11 +6920,11 @@
         <v>0</v>
       </c>
       <c r="H26" s="33">
-        <v>1E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="I26" s="29">
         <f t="shared" si="100"/>
-        <v>78.614999999999995</v>
+        <v>196.53749999999999</v>
       </c>
       <c r="J26" s="33">
         <v>0.01</v>
@@ -6934,11 +6934,11 @@
         <v>786.15</v>
       </c>
       <c r="L26" s="33">
-        <v>5.0000000000000001E-3</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="M26" s="29">
         <f t="shared" si="102"/>
-        <v>393.07499999999999</v>
+        <v>589.61249999999995</v>
       </c>
       <c r="N26" s="33">
         <v>0.01</v>
@@ -6962,18 +6962,18 @@
         <v>0</v>
       </c>
       <c r="T26" s="37">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="U26" s="31">
         <f t="shared" si="106"/>
-        <v>6289.2</v>
+        <v>7075.3499999999995</v>
       </c>
       <c r="V26" s="33">
-        <v>0.12</v>
+        <v>0.04</v>
       </c>
       <c r="W26" s="31">
         <f t="shared" si="107"/>
-        <v>9433.7999999999993</v>
+        <v>3144.6</v>
       </c>
       <c r="X26" s="33">
         <v>0</v>
@@ -6983,46 +6983,46 @@
         <v>0</v>
       </c>
       <c r="Z26" s="33">
-        <v>1E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="AA26" s="29">
         <f t="shared" si="109"/>
-        <v>78.614999999999995</v>
+        <v>235.845</v>
       </c>
       <c r="AB26" s="33">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AC26" s="29">
         <f t="shared" si="110"/>
-        <v>1572.3</v>
+        <v>1965.375</v>
       </c>
       <c r="AD26" s="33">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="AE26" s="31">
         <f t="shared" si="111"/>
-        <v>1572.3</v>
+        <v>3144.6</v>
       </c>
       <c r="AF26" s="33">
-        <v>1.4999999999999999E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="AG26" s="29">
         <f t="shared" si="119"/>
-        <v>1179.2249999999999</v>
+        <v>1100.6100000000001</v>
       </c>
       <c r="AH26" s="33">
-        <v>1.0999999999999999E-2</v>
+        <v>0.01</v>
       </c>
       <c r="AI26" s="29">
         <f t="shared" si="120"/>
-        <v>864.76499999999999</v>
+        <v>786.15</v>
       </c>
       <c r="AJ26" s="33">
-        <v>3.5000000000000003E-2</v>
+        <v>0.02</v>
       </c>
       <c r="AK26" s="31">
         <f t="shared" si="112"/>
-        <v>2751.5250000000001</v>
+        <v>1572.3</v>
       </c>
       <c r="AL26" s="33">
         <v>2.5000000000000001E-2</v>
@@ -7046,11 +7046,11 @@
         <v>393.07499999999999</v>
       </c>
       <c r="AR26" s="33">
-        <v>0.38</v>
+        <v>0.41</v>
       </c>
       <c r="AS26" s="31">
         <f t="shared" si="116"/>
-        <v>29873.7</v>
+        <v>32232.149999999998</v>
       </c>
       <c r="AT26" s="33">
         <v>0</v>
@@ -7060,18 +7060,18 @@
         <v>0</v>
       </c>
       <c r="AV26" s="33">
-        <v>2E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="AW26" s="29">
         <f t="shared" si="122"/>
-        <v>157.22999999999999</v>
+        <v>628.91999999999996</v>
       </c>
       <c r="AX26" s="33">
-        <v>2E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="AY26" s="29">
         <f t="shared" si="123"/>
-        <v>157.22999999999999</v>
+        <v>550.30500000000006</v>
       </c>
       <c r="AZ26" s="33">
         <v>0</v>
@@ -7081,25 +7081,25 @@
         <v>0</v>
       </c>
       <c r="BB26" s="33">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="BC26" s="29">
         <f t="shared" si="124"/>
-        <v>1572.3</v>
+        <v>3144.6</v>
       </c>
       <c r="BD26" s="33">
-        <v>5.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="BE26" s="29">
         <f t="shared" ref="BE26" si="130">$B26*BD26</f>
-        <v>393.07499999999999</v>
+        <v>786.15</v>
       </c>
       <c r="BF26" s="33">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="BG26" s="31">
         <f t="shared" si="117"/>
-        <v>3144.6</v>
+        <v>2358.4499999999998</v>
       </c>
       <c r="BH26" s="33">
         <v>0</v>
@@ -12655,11 +12655,11 @@
         <f>IFERROR(SUM(F51,H51,J51,L51,N51,P51,R51,T51,V51,X51,Z51,AB51,AD51,AF51,AH51,AJ51,AL51,AN51,AP51,AR51,AT51,AV51,AX51,AZ51,BB51,BD51,BF51,BH51,BJ51,BL51),0)</f>
         <v>1</v>
       </c>
-      <c r="D51" s="54">
+      <c r="D51" s="53">
         <f>SUM(E52,E56,E62,E68,E86,E100,E111)</f>
         <v>1072597.8</v>
       </c>
-      <c r="E51" s="55"/>
+      <c r="E51" s="54"/>
       <c r="F51" s="32">
         <f>IFERROR(G51/$B51,0)</f>
         <v>2.526813531299273E-3</v>
@@ -29735,24 +29735,6 @@
     <sortCondition ref="A32"/>
   </sortState>
   <mergeCells count="34">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="BB1:BC1"/>
-    <mergeCell ref="BD1:BE1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D51:E51"/>
     <mergeCell ref="BH1:BI1"/>
     <mergeCell ref="BJ1:BK1"/>
     <mergeCell ref="BL1:BM1"/>
@@ -29769,6 +29751,24 @@
     <mergeCell ref="AJ1:AK1"/>
     <mergeCell ref="AD1:AE1"/>
     <mergeCell ref="AZ1:BA1"/>
+    <mergeCell ref="BB1:BC1"/>
+    <mergeCell ref="BD1:BE1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating demographcs & religion
</commit_message>
<xml_diff>
--- a/development/tools/PopulationCalculator.xlsx
+++ b/development/tools/PopulationCalculator.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/don/Documents/GitHub/Atlas-Exandria/development/tools/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1044685-adm\Git\Atlas-Exandria\development\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C780BE33-9B18-6841-928C-FBEF84B52143}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="918" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51195" windowHeight="28800" tabRatio="474"/>
   </bookViews>
   <sheets>
     <sheet name="Population" sheetId="14" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -495,7 +494,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -810,16 +809,7 @@
     <xf numFmtId="10" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="9" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -828,10 +818,13 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -846,7 +839,13 @@
     <xf numFmtId="164" fontId="1" fillId="9" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1130,219 +1129,219 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AR62" sqref="AR62"/>
+      <selection pane="bottomLeft" activeCell="AD126" sqref="AD126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="34"/>
-    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="9.1640625" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="9.1640625" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="9.1640625" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="9.1640625" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="9.1640625" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="9.1640625" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="9.1640625" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="8.33203125" style="34" customWidth="1"/>
-    <col min="15" max="15" width="9.1640625" style="30" customWidth="1"/>
-    <col min="16" max="16" width="9.1640625" style="34" customWidth="1"/>
-    <col min="17" max="17" width="9.1640625" style="30" customWidth="1"/>
-    <col min="18" max="18" width="9.1640625" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="9.1640625" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="9.1640625" style="38" customWidth="1"/>
-    <col min="21" max="21" width="9.1640625" style="30" customWidth="1"/>
-    <col min="22" max="22" width="9.1640625" style="34" customWidth="1"/>
-    <col min="23" max="23" width="9.1640625" style="30" customWidth="1"/>
-    <col min="24" max="24" width="9.1640625" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="9.1640625" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="9.1640625" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="9.1640625" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="9.1640625" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="9.1640625" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="9.1640625" style="34" customWidth="1"/>
-    <col min="31" max="31" width="9.1640625" style="30" customWidth="1"/>
-    <col min="32" max="32" width="9.1640625" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="33" width="9.1640625" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="34" max="34" width="9.1640625" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="35" max="35" width="9.1640625" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="9.1640625" style="34" customWidth="1"/>
-    <col min="37" max="37" width="9.1640625" style="30" customWidth="1"/>
-    <col min="38" max="38" width="9.1640625" style="34" customWidth="1"/>
-    <col min="39" max="39" width="9.1640625" style="30" customWidth="1"/>
-    <col min="40" max="40" width="9.1640625" style="34" customWidth="1"/>
-    <col min="41" max="41" width="9.1640625" style="30" customWidth="1"/>
-    <col min="42" max="42" width="9.1640625" style="34" customWidth="1"/>
-    <col min="43" max="43" width="9.1640625" style="30" customWidth="1"/>
-    <col min="44" max="44" width="9.1640625" style="34" customWidth="1"/>
-    <col min="45" max="45" width="9.1640625" style="30" customWidth="1"/>
-    <col min="46" max="46" width="9.1640625" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="47" max="47" width="9.1640625" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="48" max="48" width="9.1640625" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="49" max="49" width="9.1640625" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="50" max="50" width="9.1640625" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="51" max="51" width="9.1640625" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="9.1640625" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="53" max="53" width="9.1640625" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="54" max="54" width="9.1640625" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="55" max="55" width="9.1640625" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="56" max="56" width="9.1640625" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="57" max="57" width="9.1640625" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="58" max="58" width="9.1640625" style="34" customWidth="1"/>
-    <col min="59" max="59" width="9.1640625" style="30" customWidth="1"/>
-    <col min="60" max="60" width="9.1640625" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="61" max="61" width="9.1640625" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="62" max="62" width="9.1640625" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="63" max="63" width="9.1640625" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="64" max="64" width="9.1640625" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="65" max="65" width="9.1640625" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="9.1640625"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="34"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="9.140625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="9.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="9.140625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="9.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="9.140625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="9.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="9.140625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="8.28515625" style="34" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="30" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="34" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="30" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="9.140625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="20" width="9.140625" style="38" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="30" customWidth="1"/>
+    <col min="22" max="22" width="9.140625" style="34" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" style="30" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="9.140625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="9.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="9.140625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="9.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="9.140625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="9.140625" style="34" customWidth="1"/>
+    <col min="31" max="31" width="9.140625" style="30" customWidth="1"/>
+    <col min="32" max="32" width="9.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="9.140625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="34" width="9.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="9.140625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="9.140625" style="34" customWidth="1"/>
+    <col min="37" max="37" width="9.140625" style="30" customWidth="1"/>
+    <col min="38" max="38" width="9.140625" style="34" customWidth="1"/>
+    <col min="39" max="39" width="9.140625" style="30" customWidth="1"/>
+    <col min="40" max="40" width="9.140625" style="34" customWidth="1"/>
+    <col min="41" max="41" width="9.140625" style="30" customWidth="1"/>
+    <col min="42" max="42" width="9.140625" style="34" customWidth="1"/>
+    <col min="43" max="43" width="9.140625" style="30" customWidth="1"/>
+    <col min="44" max="44" width="9.140625" style="34" customWidth="1"/>
+    <col min="45" max="45" width="9.140625" style="30" customWidth="1"/>
+    <col min="46" max="46" width="9.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="47" max="47" width="9.140625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="48" max="48" width="9.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="49" max="49" width="9.140625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="50" max="50" width="9.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="51" max="51" width="9.140625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="9.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="53" max="53" width="9.140625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="54" max="54" width="9.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="55" max="55" width="9.140625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="56" max="56" width="9.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="57" max="57" width="9.140625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="58" max="58" width="9.140625" style="34" customWidth="1"/>
+    <col min="59" max="59" width="9.140625" style="30" customWidth="1"/>
+    <col min="60" max="60" width="9.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="61" max="61" width="9.140625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="62" width="9.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="63" max="63" width="9.140625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="64" max="64" width="9.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="65" max="65" width="9.140625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="66" max="66" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" s="12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:65" s="12" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="43">
+      <c r="B1" s="53">
         <f>SUM(B51,B2)</f>
         <v>2524854</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="50">
+      <c r="C1" s="48"/>
+      <c r="D1" s="47">
         <f>SUM(D2,D51)</f>
         <v>2042171.4</v>
       </c>
-      <c r="E1" s="44"/>
-      <c r="F1" s="49" t="s">
+      <c r="E1" s="48"/>
+      <c r="F1" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49" t="s">
+      <c r="G1" s="43"/>
+      <c r="H1" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49" t="s">
+      <c r="I1" s="43"/>
+      <c r="J1" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49" t="s">
+      <c r="K1" s="43"/>
+      <c r="L1" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="49"/>
-      <c r="N1" s="47" t="s">
+      <c r="M1" s="43"/>
+      <c r="N1" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="48"/>
-      <c r="P1" s="47" t="s">
+      <c r="O1" s="45"/>
+      <c r="P1" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="45" t="s">
+      <c r="Q1" s="45"/>
+      <c r="R1" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="S1" s="46"/>
-      <c r="T1" s="47" t="s">
+      <c r="S1" s="55"/>
+      <c r="T1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="U1" s="48"/>
-      <c r="V1" s="47" t="s">
+      <c r="U1" s="45"/>
+      <c r="V1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="48"/>
-      <c r="X1" s="49" t="s">
+      <c r="W1" s="45"/>
+      <c r="X1" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" s="49"/>
-      <c r="Z1" s="49" t="s">
+      <c r="Y1" s="43"/>
+      <c r="Z1" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" s="49"/>
-      <c r="AB1" s="49" t="s">
+      <c r="AA1" s="43"/>
+      <c r="AB1" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="AC1" s="49"/>
-      <c r="AD1" s="47" t="s">
+      <c r="AC1" s="43"/>
+      <c r="AD1" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="AE1" s="48"/>
-      <c r="AF1" s="49" t="s">
+      <c r="AE1" s="45"/>
+      <c r="AF1" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="49"/>
-      <c r="AH1" s="45" t="s">
+      <c r="AG1" s="43"/>
+      <c r="AH1" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="47" t="s">
+      <c r="AI1" s="55"/>
+      <c r="AJ1" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="AK1" s="48"/>
-      <c r="AL1" s="47" t="s">
+      <c r="AK1" s="45"/>
+      <c r="AL1" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="AM1" s="48"/>
-      <c r="AN1" s="47" t="s">
+      <c r="AM1" s="45"/>
+      <c r="AN1" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="AO1" s="48"/>
-      <c r="AP1" s="55" t="s">
+      <c r="AO1" s="45"/>
+      <c r="AP1" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="AQ1" s="55"/>
-      <c r="AR1" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="AS1" s="48"/>
-      <c r="AT1" s="49" t="s">
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS1" s="45"/>
+      <c r="AT1" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="AU1" s="49"/>
-      <c r="AV1" s="49" t="s">
+      <c r="AU1" s="43"/>
+      <c r="AV1" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="AW1" s="49"/>
-      <c r="AX1" s="49" t="s">
+      <c r="AW1" s="43"/>
+      <c r="AX1" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="AY1" s="49"/>
-      <c r="AZ1" s="49" t="s">
+      <c r="AY1" s="43"/>
+      <c r="AZ1" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="BA1" s="49"/>
-      <c r="BB1" s="49" t="s">
+      <c r="BA1" s="43"/>
+      <c r="BB1" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="BC1" s="49"/>
-      <c r="BD1" s="49" t="s">
+      <c r="BC1" s="43"/>
+      <c r="BD1" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="BE1" s="49"/>
-      <c r="BF1" s="47" t="s">
+      <c r="BE1" s="43"/>
+      <c r="BF1" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="BG1" s="48"/>
-      <c r="BH1" s="49" t="s">
+      <c r="BG1" s="45"/>
+      <c r="BH1" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="BI1" s="49"/>
-      <c r="BJ1" s="49" t="s">
+      <c r="BI1" s="43"/>
+      <c r="BJ1" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="BK1" s="49"/>
-      <c r="BL1" s="49" t="s">
+      <c r="BK1" s="43"/>
+      <c r="BL1" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="BM1" s="49"/>
+      <c r="BM1" s="43"/>
     </row>
-    <row r="2" spans="1:65" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:65" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>17</v>
       </c>
@@ -1352,13 +1351,13 @@
       </c>
       <c r="C2" s="39">
         <f>IFERROR(SUM(F2,H2,J2,L2,N2,P2,R2,T2,V2,X2,Z2,AB2,AD2,AF2,AH2,AJ2,AL2,AN2,AP2,AR2,AT2,AV2,AX2,AZ2,BB2,BD2,BF2,BH2,BJ2,BL2),0)</f>
-        <v>1.0000000000000002</v>
-      </c>
-      <c r="D2" s="51">
+        <v>1</v>
+      </c>
+      <c r="D2" s="49">
         <f>SUM(E46,E42,E33,E27,E22,E13,E6,E3)</f>
         <v>969573.6</v>
       </c>
-      <c r="E2" s="52">
+      <c r="E2" s="50">
         <f>SUM(E46,E42,E33,E27,E22,E13,E6,E3)</f>
         <v>969573.6</v>
       </c>
@@ -1372,19 +1371,19 @@
       </c>
       <c r="H2" s="32">
         <f>IFERROR(I2/$B2,0)</f>
-        <v>3.0954825512160859E-3</v>
+        <v>3.0822725083597662E-3</v>
       </c>
       <c r="I2" s="29">
         <f>SUM(I46,I42,I33,I27,I22,I13,I6,I3)</f>
-        <v>3168.7</v>
+        <v>3155.1774999999998</v>
       </c>
       <c r="J2" s="32">
         <f>IFERROR(K2/$B2,0)</f>
-        <v>1.3380759886406817E-2</v>
+        <v>1.3347738442616783E-2</v>
       </c>
       <c r="K2" s="29">
         <f>SUM(K46,K42,K33,K27,K22,K13,K6,K3)</f>
-        <v>13697.254999999997</v>
+        <v>13663.452499999998</v>
       </c>
       <c r="L2" s="32">
         <f>IFERROR(M2/$B2,0)</f>
@@ -1396,19 +1395,19 @@
       </c>
       <c r="N2" s="35">
         <f>IFERROR(O2/$B2,0)</f>
-        <v>3.6556469819362617E-3</v>
+        <v>3.6468402866987148E-3</v>
       </c>
       <c r="O2" s="31">
         <f>SUM(O46,O42,O33,O27,O22,O13,O6,O3)</f>
-        <v>3742.114</v>
+        <v>3733.0989999999997</v>
       </c>
       <c r="P2" s="35">
         <f>IFERROR(Q2/$B2,0)</f>
-        <v>8.4164204080875073E-3</v>
+        <v>8.4208242441530506E-3</v>
       </c>
       <c r="Q2" s="31">
         <f>SUM(Q46,Q42,Q33,Q27,Q22,Q13,Q6,Q3)</f>
-        <v>8615.4940000000006</v>
+        <v>8620.0020000000022</v>
       </c>
       <c r="R2" s="32">
         <f>IFERROR(S2/$B2,0)</f>
@@ -1428,11 +1427,11 @@
       </c>
       <c r="V2" s="35">
         <f>IFERROR(W2/$B2,0)</f>
-        <v>9.0562818650460647E-2</v>
+        <v>9.0489546750705557E-2</v>
       </c>
       <c r="W2" s="31">
         <f>SUM(W46,W42,W33,W27,W22,W13,W6,W3)</f>
-        <v>92704.900999999998</v>
+        <v>92629.895999999993</v>
       </c>
       <c r="X2" s="32">
         <f>IFERROR(Y2/$B2,0)</f>
@@ -1452,59 +1451,59 @@
       </c>
       <c r="AB2" s="32">
         <f>IFERROR(AC2/$B2,0)</f>
-        <v>5.5467990617914477E-3</v>
+        <v>5.7593857488817011E-3</v>
       </c>
       <c r="AC2" s="29">
         <f>SUM(AC46,AC42,AC33,AC27,AC22,AC13,AC6,AC3)</f>
-        <v>5677.9975000000004</v>
+        <v>5895.6125000000002</v>
       </c>
       <c r="AD2" s="35">
         <f>IFERROR(AE2/$B2,0)</f>
-        <v>3.4707015951694571E-2</v>
+        <v>3.4677772643659531E-2</v>
       </c>
       <c r="AE2" s="31">
         <f>SUM(AE46,AE42,AE33,AE27,AE22,AE13,AE6,AE3)</f>
-        <v>35527.941000000006</v>
+        <v>35498.006000000008</v>
       </c>
       <c r="AF2" s="32">
         <f>IFERROR(AG2/$B2,0)</f>
-        <v>3.5736226045349352E-2</v>
+        <v>3.5816726957279471E-2</v>
       </c>
       <c r="AG2" s="29">
         <f>SUM(AG46,AG42,AG33,AG27,AG22,AG13,AG6,AG3)</f>
-        <v>36581.495000000003</v>
+        <v>36663.9</v>
       </c>
       <c r="AH2" s="32">
         <f>IFERROR(AI2/$B2,0)</f>
-        <v>2.6787490487499184E-3</v>
+        <v>2.6642910243998698E-3</v>
       </c>
       <c r="AI2" s="29">
         <f>SUM(AI46,AI42,AI33,AI27,AI22,AI13,AI6,AI3)</f>
-        <v>2742.1095</v>
+        <v>2727.3094999999998</v>
       </c>
       <c r="AJ2" s="35">
         <f>IFERROR(AK2/$B2,0)</f>
-        <v>4.6505322604437252E-2</v>
+        <v>4.6331766721730901E-2</v>
       </c>
       <c r="AK2" s="31">
         <f>SUM(AK46,AK42,AK33,AK27,AK22,AK13,AK6,AK3)</f>
-        <v>47605.313000000009</v>
+        <v>47427.652000000002</v>
       </c>
       <c r="AL2" s="35">
         <f>IFERROR(AM2/$B2,0)</f>
-        <v>2.9483143702016209E-2</v>
+        <v>2.9424329826611164E-2</v>
       </c>
       <c r="AM2" s="31">
         <f>SUM(AM46,AM42,AM33,AM27,AM22,AM13,AM6,AM3)</f>
-        <v>30180.5085</v>
+        <v>30120.303499999998</v>
       </c>
       <c r="AN2" s="35">
         <f>IFERROR(AO2/$B2,0)</f>
-        <v>5.1525062692142749E-2</v>
+        <v>5.1481034100422707E-2</v>
       </c>
       <c r="AO2" s="31">
         <f>SUM(AO46,AO42,AO33,AO27,AO22,AO13,AO6,AO3)</f>
-        <v>52743.785000000003</v>
+        <v>52698.715000000004</v>
       </c>
       <c r="AP2" s="35">
         <f>IFERROR(AQ2/$B2,0)</f>
@@ -1516,11 +1515,11 @@
       </c>
       <c r="AR2" s="35">
         <f>IFERROR(AS2/$B2,0)</f>
-        <v>0.36642730007141094</v>
+        <v>0.36613552150973033</v>
       </c>
       <c r="AS2" s="31">
         <f>SUM(AS46,AS42,AS33,AS27,AS22,AS13,AS6,AS3)</f>
-        <v>375094.40500000003</v>
+        <v>374795.72499999998</v>
       </c>
       <c r="AT2" s="32">
         <f>IFERROR(AU2/$B2,0)</f>
@@ -1532,19 +1531,19 @@
       </c>
       <c r="AV2" s="32">
         <f>IFERROR(AW2/$B2,0)</f>
-        <v>9.2810991615322781E-3</v>
+        <v>9.2659866185123303E-3</v>
       </c>
       <c r="AW2" s="29">
         <f>SUM(AW46,AW42,AW33,AW27,AW22,AW13,AW6,AW3)</f>
-        <v>9500.6250000000018</v>
+        <v>9485.1550000000025</v>
       </c>
       <c r="AX2" s="32">
         <f>IFERROR(AY2/$B2,0)</f>
-        <v>9.225078713196758E-3</v>
+        <v>9.4665814489871079E-3</v>
       </c>
       <c r="AY2" s="29">
         <f>SUM(AY46,AY42,AY33,AY27,AY22,AY13,AY6,AY3)</f>
-        <v>9443.2795000000006</v>
+        <v>9690.4945000000007</v>
       </c>
       <c r="AZ2" s="32">
         <f>IFERROR(BA2/$B2,0)</f>
@@ -1556,11 +1555,11 @@
       </c>
       <c r="BB2" s="32">
         <f>IFERROR(BC2/$B2,0)</f>
-        <v>1.8532928638904003E-2</v>
+        <v>1.8869390310974524E-2</v>
       </c>
       <c r="BC2" s="29">
         <f>SUM(BC46,BC42,BC33,BC27,BC22,BC13,BC6,BC3)</f>
-        <v>18971.288</v>
+        <v>19315.708000000002</v>
       </c>
       <c r="BD2" s="32">
         <f>IFERROR(BE2/$B2,0)</f>
@@ -1572,19 +1571,19 @@
       </c>
       <c r="BF2" s="35">
         <f>IFERROR(BG2/$B2,0)</f>
-        <v>3.3356791803472466E-2</v>
+        <v>3.3187906448767304E-2</v>
       </c>
       <c r="BG2" s="31">
         <f>SUM(BG46,BG42,BG33,BG27,BG22,BG13,BG6,BG3)</f>
-        <v>34145.78</v>
+        <v>33972.899999999994</v>
       </c>
       <c r="BH2" s="32">
         <f>IFERROR(BI2/$B2,0)</f>
-        <v>6.3014908372270692E-4</v>
+        <v>6.5906513242280354E-4</v>
       </c>
       <c r="BI2" s="29">
         <f>SUM(BI46,BI42,BI33,BI27,BI22,BI13,BI6,BI3)</f>
-        <v>645.05400000000009</v>
+        <v>674.65400000000011</v>
       </c>
       <c r="BJ2" s="32">
         <f>IFERROR(BK2/$B2,0)</f>
@@ -1596,14 +1595,14 @@
       </c>
       <c r="BL2" s="32">
         <f>IFERROR(BM2/$B2,0)</f>
-        <v>7.4510571453412439E-4</v>
+        <v>7.6492004614845072E-4</v>
       </c>
       <c r="BM2" s="29">
         <f>SUM(BM46,BM42,BM33,BM27,BM22,BM13,BM6,BM3)</f>
-        <v>762.72969999999998</v>
+        <v>783.0127</v>
       </c>
     </row>
-    <row r="3" spans="1:65" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>41</v>
       </c>
@@ -1863,7 +1862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -2087,7 +2086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>77</v>
       </c>
@@ -2311,7 +2310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:65" ht="16" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:65" ht="15.75" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>42</v>
       </c>
@@ -2571,7 +2570,7 @@
         <v>503.21249999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -2795,7 +2794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>79</v>
       </c>
@@ -3019,7 +3018,7 @@
         <v>287.55</v>
       </c>
     </row>
-    <row r="9" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>76</v>
       </c>
@@ -3243,7 +3242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -3467,7 +3466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>80</v>
       </c>
@@ -3691,7 +3690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>78</v>
       </c>
@@ -3915,7 +3914,7 @@
         <v>215.66249999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:65" ht="14" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:65" ht="14.1" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>46</v>
       </c>
@@ -4175,7 +4174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>81</v>
       </c>
@@ -4399,7 +4398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -4623,7 +4622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -4847,7 +4846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -5071,7 +5070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>6</v>
       </c>
@@ -5295,7 +5294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -5519,7 +5518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>69</v>
       </c>
@@ -5743,7 +5742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>82</v>
       </c>
@@ -5967,7 +5966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:65" ht="16" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:65" ht="15.75" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>47</v>
       </c>
@@ -6227,7 +6226,7 @@
         <v>85.4542</v>
       </c>
     </row>
-    <row r="23" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
@@ -6451,7 +6450,7 @@
         <v>1.5982000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
@@ -6675,7 +6674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>53</v>
       </c>
@@ -6899,7 +6898,7 @@
         <v>5.2410000000000005</v>
       </c>
     </row>
-    <row r="26" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>83</v>
       </c>
@@ -7123,7 +7122,7 @@
         <v>78.614999999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:65" ht="16" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:65" ht="15.75" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>48</v>
       </c>
@@ -7152,19 +7151,19 @@
       </c>
       <c r="H27" s="32">
         <f>IFERROR(I27/$B27,0)</f>
-        <v>1.3478300677531587E-2</v>
+        <v>1.2652902398828055E-2</v>
       </c>
       <c r="I27" s="29">
         <f>SUM(I28:I32)</f>
-        <v>220.815</v>
+        <v>207.29250000000002</v>
       </c>
       <c r="J27" s="32">
         <f>IFERROR(K27/$B27,0)</f>
-        <v>8.2530672038088268E-3</v>
+        <v>6.1898004028566192E-3</v>
       </c>
       <c r="K27" s="29">
         <f>SUM(K28:K32)</f>
-        <v>135.21</v>
+        <v>101.4075</v>
       </c>
       <c r="L27" s="32">
         <f>IFERROR(M27/$B27,0)</f>
@@ -7176,19 +7175,19 @@
       </c>
       <c r="N27" s="35">
         <f>IFERROR(O27/$B27,0)</f>
-        <v>1.4436916315693098E-2</v>
+        <v>1.3886650796557407E-2</v>
       </c>
       <c r="O27" s="31">
         <f>SUM(O28:O32)</f>
-        <v>236.52</v>
+        <v>227.505</v>
       </c>
       <c r="P27" s="35">
         <f>IFERROR(Q27/$B27,0)</f>
-        <v>2.7510224012696085E-4</v>
+        <v>5.5026551913568949E-4</v>
       </c>
       <c r="Q27" s="31">
         <f>SUM(Q28:Q32)</f>
-        <v>4.5069999999999997</v>
+        <v>9.0150000000000006</v>
       </c>
       <c r="R27" s="32">
         <f>IFERROR(S27/$B27,0)</f>
@@ -7208,11 +7207,11 @@
       </c>
       <c r="V27" s="35">
         <f>IFERROR(W27/$B27,0)</f>
-        <v>6.6968809131416715E-2</v>
+        <v>6.2842275529512298E-2</v>
       </c>
       <c r="W27" s="31">
         <f>SUM(W28:W32)</f>
-        <v>1097.1500000000001</v>
+        <v>1029.5450000000001</v>
       </c>
       <c r="X27" s="32">
         <f>IFERROR(Y27/$B27,0)</f>
@@ -7232,27 +7231,27 @@
       </c>
       <c r="AB27" s="32">
         <f>IFERROR(AC27/$B27,0)</f>
-        <v>1.0018922053347984E-2</v>
+        <v>2.2398522859061222E-2</v>
       </c>
       <c r="AC27" s="29">
         <f>SUM(AC28:AC32)</f>
-        <v>164.14000000000001</v>
+        <v>366.95499999999998</v>
       </c>
       <c r="AD27" s="35">
         <f>IFERROR(AE27/$B27,0)</f>
-        <v>1.5707135445278641E-2</v>
+        <v>1.4331624244643836E-2</v>
       </c>
       <c r="AE27" s="31">
         <f>SUM(AE28:AE32)</f>
-        <v>257.33</v>
+        <v>234.79499999999996</v>
       </c>
       <c r="AF27" s="32">
         <f>IFERROR(AG27/$B27,0)</f>
-        <v>6.0523103216749072E-3</v>
+        <v>1.0178843923579319E-2</v>
       </c>
       <c r="AG27" s="29">
         <f>SUM(AG28:AG32)</f>
-        <v>99.155000000000001</v>
+        <v>166.76</v>
       </c>
       <c r="AH27" s="32">
         <f>IFERROR(AI27/$B27,0)</f>
@@ -7264,27 +7263,27 @@
       </c>
       <c r="AJ27" s="35">
         <f>IFERROR(AK27/$B27,0)</f>
-        <v>5.948245132149179E-2</v>
+        <v>5.3155099798571685E-2</v>
       </c>
       <c r="AK27" s="31">
         <f>SUM(AK28:AK32)</f>
-        <v>974.50099999999998</v>
+        <v>870.83999999999992</v>
       </c>
       <c r="AL27" s="35">
         <f>IFERROR(AM27/$B27,0)</f>
-        <v>1.9471708478300678E-2</v>
+        <v>1.5345174876396264E-2</v>
       </c>
       <c r="AM27" s="31">
         <f>SUM(AM28:AM32)</f>
-        <v>319.005</v>
+        <v>251.4</v>
       </c>
       <c r="AN27" s="35">
         <f>IFERROR(AO27/$B27,0)</f>
-        <v>7.5170298480131847E-2</v>
+        <v>7.2419276078862241E-2</v>
       </c>
       <c r="AO27" s="31">
         <f>SUM(AO28:AO32)</f>
-        <v>1231.5150000000001</v>
+        <v>1186.4450000000002</v>
       </c>
       <c r="AP27" s="35">
         <f>IFERROR(AQ27/$B27,0)</f>
@@ -7296,11 +7295,11 @@
       </c>
       <c r="AR27" s="35">
         <f>IFERROR(AS27/$B27,0)</f>
-        <v>0.5669324909967649</v>
+        <v>0.55592840139168653</v>
       </c>
       <c r="AS27" s="31">
         <f>SUM(AS28:AS32)</f>
-        <v>9288.0550000000003</v>
+        <v>9107.7749999999996</v>
       </c>
       <c r="AT27" s="32">
         <f>IFERROR(AU27/$B27,0)</f>
@@ -7312,19 +7311,19 @@
       </c>
       <c r="AV27" s="32">
         <f>IFERROR(AW27/$B27,0)</f>
-        <v>8.2530672038088268E-3</v>
+        <v>5.5020448025392176E-3</v>
       </c>
       <c r="AW27" s="29">
         <f>SUM(AW28:AW32)</f>
-        <v>135.21</v>
+        <v>90.14</v>
       </c>
       <c r="AX27" s="32">
         <f>IFERROR(AY27/$B27,0)</f>
-        <v>1.8283586644692672E-2</v>
+        <v>3.0663187450405905E-2</v>
       </c>
       <c r="AY27" s="29">
         <f>SUM(AY28:AY32)</f>
-        <v>299.54000000000002</v>
+        <v>502.35499999999996</v>
       </c>
       <c r="AZ27" s="32">
         <f>IFERROR(BA27/$B27,0)</f>
@@ -7336,11 +7335,11 @@
       </c>
       <c r="BB27" s="32">
         <f>IFERROR(BC27/$B27,0)</f>
-        <v>1.7315815174266006E-2</v>
+        <v>3.3821949581883663E-2</v>
       </c>
       <c r="BC27" s="29">
         <f>SUM(BC28:BC32)</f>
-        <v>283.685</v>
+        <v>554.10500000000002</v>
       </c>
       <c r="BD27" s="32">
         <f>IFERROR(BE27/$B27,0)</f>
@@ -7352,11 +7351,11 @@
       </c>
       <c r="BF27" s="35">
         <f>IFERROR(BG27/$B27,0)</f>
-        <v>4.5386681315998295E-2</v>
+        <v>3.4382591710919862E-2</v>
       </c>
       <c r="BG27" s="31">
         <f>SUM(BG28:BG32)</f>
-        <v>743.57</v>
+        <v>563.29000000000008</v>
       </c>
       <c r="BH27" s="32">
         <f>IFERROR(BI27/$B27,0)</f>
@@ -7376,14 +7375,14 @@
       </c>
       <c r="BL27" s="32">
         <f>IFERROR(BM27/$B27,0)</f>
-        <v>8.2536775926265028E-4</v>
+        <v>2.0634193981566257E-3</v>
       </c>
       <c r="BM27" s="29">
         <f>SUM(BM28:BM32)</f>
-        <v>13.522</v>
+        <v>33.805</v>
       </c>
     </row>
-    <row r="28" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>18</v>
       </c>
@@ -7607,7 +7606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -7831,7 +7830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>19</v>
       </c>
@@ -7852,11 +7851,11 @@
         <v>0</v>
       </c>
       <c r="H30" s="33">
-        <v>1.9E-2</v>
+        <v>1.7500000000000002E-2</v>
       </c>
       <c r="I30" s="29">
         <f t="shared" si="132"/>
-        <v>171.285</v>
+        <v>157.76250000000002</v>
       </c>
       <c r="J30" s="33">
         <v>0</v>
@@ -7873,18 +7872,18 @@
         <v>0</v>
       </c>
       <c r="N30" s="33">
-        <v>0.02</v>
+        <v>1.9E-2</v>
       </c>
       <c r="O30" s="31">
         <f t="shared" si="135"/>
-        <v>180.3</v>
+        <v>171.285</v>
       </c>
       <c r="P30" s="33">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="Q30" s="31">
         <f t="shared" si="136"/>
-        <v>0</v>
+        <v>9.0150000000000006</v>
       </c>
       <c r="R30" s="33">
         <v>0</v>
@@ -8048,14 +8047,14 @@
         <v>0</v>
       </c>
       <c r="BL30" s="33">
-        <v>1E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="BM30" s="29">
         <f t="shared" si="160"/>
-        <v>9.0150000000000006</v>
+        <v>22.537500000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>20</v>
       </c>
@@ -8279,7 +8278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>84</v>
       </c>
@@ -8307,11 +8306,11 @@
         <v>45.07</v>
       </c>
       <c r="J32" s="33">
-        <v>0.03</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="K32" s="29">
         <f t="shared" si="133"/>
-        <v>135.21</v>
+        <v>101.4075</v>
       </c>
       <c r="L32" s="33">
         <v>0.01</v>
@@ -8328,11 +8327,11 @@
         <v>45.07</v>
       </c>
       <c r="P32" s="33">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="Q32" s="31">
         <f t="shared" si="136"/>
-        <v>4.5069999999999997</v>
+        <v>0</v>
       </c>
       <c r="R32" s="33">
         <v>0</v>
@@ -8349,11 +8348,11 @@
         <v>90.14</v>
       </c>
       <c r="V32" s="33">
-        <v>0.04</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="W32" s="31">
         <f t="shared" si="139"/>
-        <v>180.28</v>
+        <v>112.67500000000001</v>
       </c>
       <c r="X32" s="33">
         <v>0</v>
@@ -8370,25 +8369,25 @@
         <v>0</v>
       </c>
       <c r="AB32" s="33">
-        <v>0.03</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="AC32" s="29">
         <f t="shared" si="142"/>
-        <v>135.21</v>
+        <v>338.02499999999998</v>
       </c>
       <c r="AD32" s="33">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="AE32" s="31">
         <f t="shared" si="143"/>
-        <v>90.14</v>
+        <v>67.605000000000004</v>
       </c>
       <c r="AF32" s="33">
-        <v>0.02</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="AG32" s="29">
         <f t="shared" si="151"/>
-        <v>90.14</v>
+        <v>157.745</v>
       </c>
       <c r="AH32" s="33">
         <v>0.01</v>
@@ -8398,25 +8397,25 @@
         <v>45.07</v>
       </c>
       <c r="AJ32" s="33">
-        <v>4.8000000000000001E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AK32" s="31">
         <f t="shared" si="144"/>
-        <v>216.33600000000001</v>
+        <v>112.67500000000001</v>
       </c>
       <c r="AL32" s="33">
-        <v>5.5E-2</v>
+        <v>0.04</v>
       </c>
       <c r="AM32" s="31">
         <f t="shared" si="145"/>
-        <v>247.88499999999999</v>
+        <v>180.28</v>
       </c>
       <c r="AN32" s="33">
-        <v>4.4999999999999998E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="AO32" s="31">
         <f t="shared" si="146"/>
-        <v>202.815</v>
+        <v>157.745</v>
       </c>
       <c r="AP32" s="33">
         <v>0.01</v>
@@ -8426,11 +8425,11 @@
         <v>45.07</v>
       </c>
       <c r="AR32" s="33">
-        <v>0.41</v>
+        <v>0.37</v>
       </c>
       <c r="AS32" s="31">
         <f t="shared" si="148"/>
-        <v>1847.87</v>
+        <v>1667.59</v>
       </c>
       <c r="AT32" s="33">
         <v>0</v>
@@ -8440,18 +8439,18 @@
         <v>0</v>
       </c>
       <c r="AV32" s="33">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="AW32" s="29">
         <f t="shared" si="154"/>
-        <v>135.21</v>
+        <v>90.14</v>
       </c>
       <c r="AX32" s="33">
-        <v>0.06</v>
+        <v>0.105</v>
       </c>
       <c r="AY32" s="29">
         <f t="shared" si="155"/>
-        <v>270.42</v>
+        <v>473.23499999999996</v>
       </c>
       <c r="AZ32" s="33">
         <v>0</v>
@@ -8461,11 +8460,11 @@
         <v>0</v>
       </c>
       <c r="BB32" s="33">
-        <v>0.05</v>
+        <v>0.11</v>
       </c>
       <c r="BC32" s="29">
         <f t="shared" si="156"/>
-        <v>225.35000000000002</v>
+        <v>495.77</v>
       </c>
       <c r="BD32" s="33">
         <v>0.02</v>
@@ -8475,11 +8474,11 @@
         <v>90.14</v>
       </c>
       <c r="BF32" s="33">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="BG32" s="31">
         <f t="shared" si="149"/>
-        <v>225.35000000000002</v>
+        <v>45.07</v>
       </c>
       <c r="BH32" s="33">
         <v>0.02</v>
@@ -8496,14 +8495,14 @@
         <v>0</v>
       </c>
       <c r="BL32" s="33">
-        <v>1E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="BM32" s="29">
         <f t="shared" si="160"/>
-        <v>4.5069999999999997</v>
+        <v>11.2675</v>
       </c>
     </row>
-    <row r="33" spans="1:65" ht="16" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:65" ht="15.75" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>50</v>
       </c>
@@ -8763,7 +8762,7 @@
         <v>160.54100000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>13</v>
       </c>
@@ -8987,7 +8986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>74</v>
       </c>
@@ -9211,7 +9210,7 @@
         <v>2.133</v>
       </c>
     </row>
-    <row r="36" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>72</v>
       </c>
@@ -9435,7 +9434,7 @@
         <v>3.081</v>
       </c>
     </row>
-    <row r="37" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>73</v>
       </c>
@@ -9659,7 +9658,7 @@
         <v>2.6070000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>55</v>
       </c>
@@ -9883,7 +9882,7 @@
         <v>2.23</v>
       </c>
     </row>
-    <row r="39" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>71</v>
       </c>
@@ -10107,7 +10106,7 @@
         <v>3.5500000000000003</v>
       </c>
     </row>
-    <row r="40" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>54</v>
       </c>
@@ -10331,7 +10330,7 @@
         <v>4.74</v>
       </c>
     </row>
-    <row r="41" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>85</v>
       </c>
@@ -10555,7 +10554,7 @@
         <v>142.20000000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:65" ht="16" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:65" ht="15.75" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>49</v>
       </c>
@@ -10565,7 +10564,7 @@
       </c>
       <c r="C42" s="40">
         <f>IFERROR(SUM(F42,H42,J42,L42,N42,P42,R42,T42,V42,X42,Z42,AB42,AD42,AF42,AH42,AJ42,AL42,AN42,AP42,AR42,AT42,AV42,AX42,AZ42,BB42,BD42,BF42,BH42,BJ42,BL42),0)</f>
-        <v>1</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="D42" s="26">
         <v>90</v>
@@ -10640,11 +10639,11 @@
       </c>
       <c r="V42" s="35">
         <f>IFERROR(W42/$B42,0)</f>
-        <v>1.2080989876265467E-2</v>
+        <v>1.1248593925759279E-2</v>
       </c>
       <c r="W42" s="31">
         <f>SUM(W43:W45)</f>
-        <v>107.4</v>
+        <v>100</v>
       </c>
       <c r="X42" s="32">
         <f>IFERROR(Y42/$B42,0)</f>
@@ -10664,51 +10663,51 @@
       </c>
       <c r="AB42" s="32">
         <f>IFERROR(AC42/$B42,0)</f>
-        <v>6.6591676040494941E-3</v>
+        <v>8.3239595050618679E-3</v>
       </c>
       <c r="AC42" s="29">
         <f>SUM(AC43:AC45)</f>
-        <v>59.2</v>
+        <v>74</v>
       </c>
       <c r="AD42" s="35">
         <f>IFERROR(AE42/$B42,0)</f>
-        <v>3.951181102362205E-2</v>
+        <v>3.8679415073115855E-2</v>
       </c>
       <c r="AE42" s="31">
         <f>SUM(AE43:AE45)</f>
-        <v>351.26</v>
+        <v>343.85999999999996</v>
       </c>
       <c r="AF42" s="32">
         <f>IFERROR(AG42/$B42,0)</f>
-        <v>1.6647919010123736E-2</v>
+        <v>1.831271091113611E-2</v>
       </c>
       <c r="AG42" s="29">
         <f>SUM(AG43:AG45)</f>
-        <v>148</v>
+        <v>162.80000000000001</v>
       </c>
       <c r="AH42" s="32">
         <f>IFERROR(AI42/$B42,0)</f>
-        <v>4.9943757030371204E-3</v>
+        <v>3.3295838020247471E-3</v>
       </c>
       <c r="AI42" s="29">
         <f>SUM(AI43:AI45)</f>
-        <v>44.4</v>
+        <v>29.6</v>
       </c>
       <c r="AJ42" s="35">
         <f>IFERROR(AK42/$B42,0)</f>
-        <v>3.3717660292463439E-2</v>
+        <v>2.5393700787401576E-2</v>
       </c>
       <c r="AK42" s="31">
         <f>SUM(AK43:AK45)</f>
-        <v>299.75</v>
+        <v>225.75</v>
       </c>
       <c r="AL42" s="35">
         <f>IFERROR(AM42/$B42,0)</f>
-        <v>8.3239595050618677E-4</v>
+        <v>1.6647919010123735E-3</v>
       </c>
       <c r="AM42" s="31">
         <f>SUM(AM43:AM45)</f>
-        <v>7.4</v>
+        <v>14.8</v>
       </c>
       <c r="AN42" s="35">
         <f>IFERROR(AO42/$B42,0)</f>
@@ -10728,11 +10727,11 @@
       </c>
       <c r="AR42" s="35">
         <f>IFERROR(AS42/$B42,0)</f>
-        <v>0.11029808773903263</v>
+        <v>9.6979752530933647E-2</v>
       </c>
       <c r="AS42" s="31">
         <f>SUM(AS43:AS45)</f>
-        <v>980.55000000000007</v>
+        <v>862.15000000000009</v>
       </c>
       <c r="AT42" s="32">
         <f>IFERROR(AU42/$B42,0)</f>
@@ -10744,19 +10743,19 @@
       </c>
       <c r="AV42" s="32">
         <f>IFERROR(AW42/$B42,0)</f>
-        <v>1.831271091113611E-2</v>
+        <v>2.1642294713160856E-2</v>
       </c>
       <c r="AW42" s="29">
         <f>SUM(AW43:AW45)</f>
-        <v>162.80000000000001</v>
+        <v>192.4</v>
       </c>
       <c r="AX42" s="32">
         <f>IFERROR(AY42/$B42,0)</f>
-        <v>1.4150731158605176E-2</v>
+        <v>1.9145106861642298E-2</v>
       </c>
       <c r="AY42" s="29">
         <f>SUM(AY43:AY45)</f>
-        <v>125.80000000000001</v>
+        <v>170.20000000000002</v>
       </c>
       <c r="AZ42" s="32">
         <f>IFERROR(BA42/$B42,0)</f>
@@ -10768,11 +10767,11 @@
       </c>
       <c r="BB42" s="32">
         <f>IFERROR(BC42/$B42,0)</f>
-        <v>1.4983127109111359E-2</v>
+        <v>2.3307086614173231E-2</v>
       </c>
       <c r="BC42" s="29">
         <f>SUM(BC43:BC45)</f>
-        <v>133.19999999999999</v>
+        <v>207.20000000000002</v>
       </c>
       <c r="BD42" s="32">
         <f>IFERROR(BE42/$B42,0)</f>
@@ -10784,19 +10783,19 @@
       </c>
       <c r="BF42" s="35">
         <f>IFERROR(BG42/$B42,0)</f>
-        <v>4.5838020247469064E-3</v>
+        <v>5.4161979752530929E-3</v>
       </c>
       <c r="BG42" s="31">
         <f>SUM(BG43:BG45)</f>
-        <v>40.75</v>
+        <v>48.15</v>
       </c>
       <c r="BH42" s="32">
         <f>IFERROR(BI42/$B42,0)</f>
-        <v>4.9943757030371213E-3</v>
+        <v>8.3239595050618679E-3</v>
       </c>
       <c r="BI42" s="29">
         <f>SUM(BI43:BI45)</f>
-        <v>44.400000000000006</v>
+        <v>74</v>
       </c>
       <c r="BJ42" s="32">
         <f>IFERROR(BK42/$B42,0)</f>
@@ -10815,7 +10814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>12</v>
       </c>
@@ -11039,7 +11038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>70</v>
       </c>
@@ -11263,7 +11262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>86</v>
       </c>
@@ -11272,7 +11271,7 @@
       </c>
       <c r="C45" s="40">
         <f t="shared" si="219"/>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="D45" s="15"/>
       <c r="E45" s="16"/>
@@ -11333,11 +11332,11 @@
         <v>14.8</v>
       </c>
       <c r="V45" s="33">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="W45" s="31">
         <f t="shared" si="208"/>
-        <v>29.6</v>
+        <v>22.2</v>
       </c>
       <c r="X45" s="33">
         <v>0</v>
@@ -11354,46 +11353,46 @@
         <v>0</v>
       </c>
       <c r="AB45" s="33">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="AC45" s="29">
         <f t="shared" si="211"/>
-        <v>59.2</v>
+        <v>74</v>
       </c>
       <c r="AD45" s="33">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AE45" s="31">
         <f t="shared" si="212"/>
-        <v>14.8</v>
+        <v>7.4</v>
       </c>
       <c r="AF45" s="33">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="AG45" s="29">
         <f t="shared" si="220"/>
-        <v>148</v>
+        <v>162.80000000000001</v>
       </c>
       <c r="AH45" s="33">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="AI45" s="29">
         <f t="shared" si="221"/>
-        <v>44.4</v>
+        <v>29.6</v>
       </c>
       <c r="AJ45" s="33">
-        <v>0.09</v>
+        <v>0.04</v>
       </c>
       <c r="AK45" s="31">
         <f t="shared" si="213"/>
-        <v>133.19999999999999</v>
+        <v>59.2</v>
       </c>
       <c r="AL45" s="33">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AM45" s="31">
         <f t="shared" si="214"/>
-        <v>0</v>
+        <v>7.4</v>
       </c>
       <c r="AN45" s="33">
         <v>4.4999999999999998E-2</v>
@@ -11410,11 +11409,11 @@
         <v>0</v>
       </c>
       <c r="AR45" s="33">
-        <v>0.32</v>
+        <v>0.24</v>
       </c>
       <c r="AS45" s="31">
         <f t="shared" si="217"/>
-        <v>473.6</v>
+        <v>355.2</v>
       </c>
       <c r="AT45" s="33">
         <v>0</v>
@@ -11424,18 +11423,18 @@
         <v>0</v>
       </c>
       <c r="AV45" s="33">
-        <v>0.11</v>
+        <v>0.13</v>
       </c>
       <c r="AW45" s="29">
         <f t="shared" si="223"/>
-        <v>162.80000000000001</v>
+        <v>192.4</v>
       </c>
       <c r="AX45" s="33">
-        <v>0.08</v>
+        <v>0.11</v>
       </c>
       <c r="AY45" s="29">
         <f t="shared" si="224"/>
-        <v>118.4</v>
+        <v>162.80000000000001</v>
       </c>
       <c r="AZ45" s="33">
         <v>0</v>
@@ -11445,11 +11444,11 @@
         <v>0</v>
       </c>
       <c r="BB45" s="33">
-        <v>0.09</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="BC45" s="29">
         <f t="shared" si="225"/>
-        <v>133.19999999999999</v>
+        <v>207.20000000000002</v>
       </c>
       <c r="BD45" s="33">
         <v>0.01</v>
@@ -11459,18 +11458,18 @@
         <v>14.8</v>
       </c>
       <c r="BF45" s="33">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="BG45" s="31">
         <f t="shared" si="218"/>
-        <v>0</v>
+        <v>7.4</v>
       </c>
       <c r="BH45" s="33">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="BI45" s="29">
         <f t="shared" si="227"/>
-        <v>29.6</v>
+        <v>59.2</v>
       </c>
       <c r="BJ45" s="33">
         <v>0</v>
@@ -11487,7 +11486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:65" ht="16" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:65" ht="15.75" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>51</v>
       </c>
@@ -11747,7 +11746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>15</v>
       </c>
@@ -11971,7 +11970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>14</v>
       </c>
@@ -12195,7 +12194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>75</v>
       </c>
@@ -12419,7 +12418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>87</v>
       </c>
@@ -12643,7 +12642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:65" ht="19" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:65" ht="18.75" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
         <v>61</v>
       </c>
@@ -12655,11 +12654,11 @@
         <f>IFERROR(SUM(F51,H51,J51,L51,N51,P51,R51,T51,V51,X51,Z51,AB51,AD51,AF51,AH51,AJ51,AL51,AN51,AP51,AR51,AT51,AV51,AX51,AZ51,BB51,BD51,BF51,BH51,BJ51,BL51),0)</f>
         <v>1</v>
       </c>
-      <c r="D51" s="53">
+      <c r="D51" s="51">
         <f>SUM(E52,E56,E62,E68,E86,E100,E111)</f>
         <v>1072597.8</v>
       </c>
-      <c r="E51" s="54"/>
+      <c r="E51" s="52"/>
       <c r="F51" s="32">
         <f>IFERROR(G51/$B51,0)</f>
         <v>2.526813531299273E-3</v>
@@ -12901,7 +12900,7 @@
         <v>667.81999999999994</v>
       </c>
     </row>
-    <row r="52" spans="1:65" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>62</v>
       </c>
@@ -13161,7 +13160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>152</v>
       </c>
@@ -13385,7 +13384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>153</v>
       </c>
@@ -13609,7 +13608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>154</v>
       </c>
@@ -13833,7 +13832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:65" ht="16" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:65" ht="15.75" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>63</v>
       </c>
@@ -14093,7 +14092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>137</v>
       </c>
@@ -14317,7 +14316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>138</v>
       </c>
@@ -14541,7 +14540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>139</v>
       </c>
@@ -14765,7 +14764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>140</v>
       </c>
@@ -14989,7 +14988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>141</v>
       </c>
@@ -15213,7 +15212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:65" ht="16" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:65" ht="15.75" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>64</v>
       </c>
@@ -15473,7 +15472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>132</v>
       </c>
@@ -15697,7 +15696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>133</v>
       </c>
@@ -15921,7 +15920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>134</v>
       </c>
@@ -16145,7 +16144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>135</v>
       </c>
@@ -16369,7 +16368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>136</v>
       </c>
@@ -16593,7 +16592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:65" ht="16" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:65" ht="15.75" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>65</v>
       </c>
@@ -16853,7 +16852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>101</v>
       </c>
@@ -17077,7 +17076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>102</v>
       </c>
@@ -17301,7 +17300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>103</v>
       </c>
@@ -17525,7 +17524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>104</v>
       </c>
@@ -17749,7 +17748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>105</v>
       </c>
@@ -17973,7 +17972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>106</v>
       </c>
@@ -18197,7 +18196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>107</v>
       </c>
@@ -18421,7 +18420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>109</v>
       </c>
@@ -18645,7 +18644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>108</v>
       </c>
@@ -18869,7 +18868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>110</v>
       </c>
@@ -19093,7 +19092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>111</v>
       </c>
@@ -19317,7 +19316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>112</v>
       </c>
@@ -19541,7 +19540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>113</v>
       </c>
@@ -19765,7 +19764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>114</v>
       </c>
@@ -19989,7 +19988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>115</v>
       </c>
@@ -20213,7 +20212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>116</v>
       </c>
@@ -20437,7 +20436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>117</v>
       </c>
@@ -20661,7 +20660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:65" ht="16" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:65" ht="15.75" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>66</v>
       </c>
@@ -20921,7 +20920,7 @@
         <v>637.04</v>
       </c>
     </row>
-    <row r="87" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>88</v>
       </c>
@@ -21145,7 +21144,7 @@
         <v>0.79800000000000004</v>
       </c>
     </row>
-    <row r="88" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>89</v>
       </c>
@@ -21369,7 +21368,7 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="89" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>90</v>
       </c>
@@ -21593,7 +21592,7 @@
         <v>2.6120000000000001</v>
       </c>
     </row>
-    <row r="90" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>91</v>
       </c>
@@ -21817,7 +21816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>92</v>
       </c>
@@ -22041,7 +22040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>93</v>
       </c>
@@ -22265,7 +22264,7 @@
         <v>63.800000000000004</v>
       </c>
     </row>
-    <row r="93" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>96</v>
       </c>
@@ -22489,7 +22488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>97</v>
       </c>
@@ -22713,7 +22712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>98</v>
       </c>
@@ -22937,7 +22936,7 @@
         <v>82.11</v>
       </c>
     </row>
-    <row r="96" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>99</v>
       </c>
@@ -23161,7 +23160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>100</v>
       </c>
@@ -23385,7 +23384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>94</v>
       </c>
@@ -23609,7 +23608,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="99" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>95</v>
       </c>
@@ -23833,7 +23832,7 @@
         <v>167.2</v>
       </c>
     </row>
-    <row r="100" spans="1:65" ht="16" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:65" ht="15.75" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>67</v>
       </c>
@@ -24093,7 +24092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>142</v>
       </c>
@@ -24317,7 +24316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>144</v>
       </c>
@@ -24541,7 +24540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>145</v>
       </c>
@@ -24765,7 +24764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>146</v>
       </c>
@@ -24989,7 +24988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>147</v>
       </c>
@@ -25213,7 +25212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>148</v>
       </c>
@@ -25437,7 +25436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>149</v>
       </c>
@@ -25661,7 +25660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>150</v>
       </c>
@@ -25885,7 +25884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>151</v>
       </c>
@@ -26109,7 +26108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>143</v>
       </c>
@@ -26333,7 +26332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:65" ht="16" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:65" ht="15.75" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>68</v>
       </c>
@@ -26593,7 +26592,7 @@
         <v>30.78</v>
       </c>
     </row>
-    <row r="112" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>118</v>
       </c>
@@ -26817,7 +26816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>119</v>
       </c>
@@ -27041,7 +27040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>120</v>
       </c>
@@ -27265,7 +27264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>121</v>
       </c>
@@ -27489,7 +27488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>122</v>
       </c>
@@ -27713,7 +27712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>123</v>
       </c>
@@ -27937,7 +27936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>124</v>
       </c>
@@ -28161,7 +28160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>125</v>
       </c>
@@ -28385,7 +28384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>126</v>
       </c>
@@ -28609,7 +28608,7 @@
         <v>20.52</v>
       </c>
     </row>
-    <row r="121" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>127</v>
       </c>
@@ -28833,7 +28832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>128</v>
       </c>
@@ -29057,7 +29056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>129</v>
       </c>
@@ -29281,7 +29280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>130</v>
       </c>
@@ -29505,7 +29504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:65" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>131</v>
       </c>
@@ -29729,12 +29728,30 @@
         <v>10.26</v>
       </c>
     </row>
-    <row r="126" spans="1:65" collapsed="1" x14ac:dyDescent="0.2"/>
+    <row r="126" spans="1:65" collapsed="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sortState ref="A32:A34">
     <sortCondition ref="A32"/>
   </sortState>
   <mergeCells count="34">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="BB1:BC1"/>
+    <mergeCell ref="BD1:BE1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D51:E51"/>
     <mergeCell ref="BH1:BI1"/>
     <mergeCell ref="BJ1:BK1"/>
     <mergeCell ref="BL1:BM1"/>
@@ -29751,24 +29768,6 @@
     <mergeCell ref="AJ1:AK1"/>
     <mergeCell ref="AD1:AE1"/>
     <mergeCell ref="AZ1:BA1"/>
-    <mergeCell ref="BB1:BC1"/>
-    <mergeCell ref="BD1:BE1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>